<commit_message>
Fixed Glossary region gen
</commit_message>
<xml_diff>
--- a/Templates/SIOP-RSLIL-v2.1.xlsx
+++ b/Templates/SIOP-RSLIL-v2.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="841">
   <si>
     <t>Id</t>
   </si>
@@ -8844,7 +8844,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -9843,8 +9843,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10535,7 +10535,9 @@
       <c r="C34" s="15" t="s">
         <v>424</v>
       </c>
-      <c r="D34" s="15"/>
+      <c r="D34" s="15" t="s">
+        <v>799</v>
+      </c>
       <c r="E34" s="15"/>
       <c r="F34" s="15" t="s">
         <v>807</v>

</xml_diff>

<commit_message>
Fixed Goal region gen
</commit_message>
<xml_diff>
--- a/Templates/SIOP-RSLIL-v2.1.xlsx
+++ b/Templates/SIOP-RSLIL-v2.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="841">
   <si>
     <t>Id</t>
   </si>
@@ -9109,7 +9109,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10821,8 +10821,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11415,10 +11415,10 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N97"/>
+  <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11501,7 +11501,7 @@
       <c r="E9" s="113"/>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1">
-      <c r="I10" s="2"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1">
       <c r="A11" s="199" t="s">
@@ -13679,10 +13679,149 @@
       <c r="M97" s="23"/>
       <c r="N97" s="23"/>
     </row>
+    <row r="99" spans="1:14">
+      <c r="A99" s="199" t="s">
+        <v>509</v>
+      </c>
+      <c r="B99" s="200"/>
+    </row>
+    <row r="100" spans="1:14" ht="47.25">
+      <c r="A100" s="79" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="79" t="s">
+        <v>181</v>
+      </c>
+      <c r="E100" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="F100" s="137" t="s">
+        <v>564</v>
+      </c>
+      <c r="G100" s="137" t="s">
+        <v>565</v>
+      </c>
+      <c r="H100" s="157" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" s="197" t="s">
+        <v>613</v>
+      </c>
+      <c r="B101" s="197"/>
+      <c r="C101" s="197"/>
+      <c r="D101" s="197"/>
+      <c r="E101" s="197"/>
+      <c r="F101" s="197"/>
+      <c r="G101" s="197"/>
+      <c r="H101" s="269"/>
+    </row>
+    <row r="102" spans="1:14" ht="30">
+      <c r="A102" s="146" t="s">
+        <v>568</v>
+      </c>
+      <c r="B102" s="145" t="s">
+        <v>625</v>
+      </c>
+      <c r="C102" s="143" t="s">
+        <v>601</v>
+      </c>
+      <c r="D102" s="143" t="str">
+        <f>stakeholders!A$21</f>
+        <v>stk.administradorsistema</v>
+      </c>
+      <c r="E102" s="143" t="s">
+        <v>254</v>
+      </c>
+      <c r="F102" s="144"/>
+      <c r="G102" s="144"/>
+      <c r="H102" s="14"/>
+    </row>
+    <row r="103" spans="1:14" ht="30">
+      <c r="A103" s="139" t="s">
+        <v>569</v>
+      </c>
+      <c r="B103" s="139" t="s">
+        <v>567</v>
+      </c>
+      <c r="C103" s="139" t="s">
+        <v>610</v>
+      </c>
+      <c r="D103" s="139" t="str">
+        <f>stakeholders!A$21</f>
+        <v>stk.administradorsistema</v>
+      </c>
+      <c r="E103" s="139" t="s">
+        <v>254</v>
+      </c>
+      <c r="F103" s="140" t="str">
+        <f>A102</f>
+        <v>G.CC</v>
+      </c>
+      <c r="G103" s="140"/>
+      <c r="H103" s="14"/>
+    </row>
+    <row r="104" spans="1:14" ht="30">
+      <c r="A104" s="138" t="s">
+        <v>602</v>
+      </c>
+      <c r="B104" s="138" t="s">
+        <v>603</v>
+      </c>
+      <c r="C104" s="138" t="s">
+        <v>686</v>
+      </c>
+      <c r="D104" s="138" t="str">
+        <f>stakeholders!A$21</f>
+        <v>stk.administradorsistema</v>
+      </c>
+      <c r="E104" s="138" t="s">
+        <v>254</v>
+      </c>
+      <c r="F104" s="18" t="str">
+        <f>A103</f>
+        <v>G.CC.1</v>
+      </c>
+      <c r="G104" s="18"/>
+      <c r="H104" s="14"/>
+    </row>
+    <row r="105" spans="1:14" ht="30">
+      <c r="A105" s="138" t="s">
+        <v>604</v>
+      </c>
+      <c r="B105" s="138" t="s">
+        <v>611</v>
+      </c>
+      <c r="C105" s="138" t="s">
+        <v>612</v>
+      </c>
+      <c r="D105" s="138" t="str">
+        <f>stakeholders!A$21</f>
+        <v>stk.administradorsistema</v>
+      </c>
+      <c r="E105" s="138" t="s">
+        <v>253</v>
+      </c>
+      <c r="F105" s="18" t="str">
+        <f>A103</f>
+        <v>G.CC.1</v>
+      </c>
+      <c r="G105" s="18"/>
+      <c r="H105" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
     <mergeCell ref="A87:H87"/>
     <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A101:H101"/>
     <mergeCell ref="C7:D8"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -13699,10 +13838,10 @@
     <mergeCell ref="A75:H75"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E95:E97 E63:E74 E41:E61 E76:E86 E88:E90 E30:E39 E14:E28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E95:E97 E63:E74 E41:E61 E76:E86 E88:E90 E30:E39 E14:E28 E102:E105">
       <formula1>CriticalityGoal</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H95:H97 H14:H28 H30:H39 H41:H61 H63:H74 H76:H86 H88:H90">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H95:H97 H14:H28 H30:H39 H41:H61 H63:H74 H76:H86 H88:H90 H102:H105">
       <formula1>ProgressState</formula1>
     </dataValidation>
   </dataValidations>
@@ -13718,7 +13857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed the Requirements sheets
</commit_message>
<xml_diff>
--- a/Templates/SIOP-RSLIL-v2.1.xlsx
+++ b/Templates/SIOP-RSLIL-v2.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -3702,324 +3702,6 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4037,6 +3719,324 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -4474,7 +4474,7 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
@@ -4498,29 +4498,29 @@
       <c r="C1" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
     </row>
     <row r="4" spans="1:8" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>471</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="90" t="s">
@@ -4534,40 +4534,40 @@
     </row>
     <row r="8" spans="1:8" ht="39" customHeight="1"/>
     <row r="9" spans="1:8">
-      <c r="A9" s="239" t="s">
+      <c r="A9" s="219" t="s">
         <v>482</v>
       </c>
-      <c r="B9" s="240"/>
-      <c r="C9" s="240"/>
-      <c r="D9" s="240"/>
-      <c r="E9" s="240"/>
-      <c r="F9" s="240"/>
-      <c r="G9" s="240"/>
-      <c r="H9" s="241"/>
+      <c r="B9" s="220"/>
+      <c r="C9" s="220"/>
+      <c r="D9" s="220"/>
+      <c r="E9" s="220"/>
+      <c r="F9" s="220"/>
+      <c r="G9" s="220"/>
+      <c r="H9" s="221"/>
     </row>
     <row r="10" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A10" s="266" t="s">
+      <c r="A10" s="160" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="266" t="s">
+      <c r="B10" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="266" t="s">
+      <c r="C10" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="266" t="s">
+      <c r="D10" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="266" t="s">
+      <c r="E10" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="266" t="s">
+      <c r="F10" s="160" t="s">
         <v>169</v>
       </c>
-      <c r="G10" s="266" t="s">
+      <c r="G10" s="160" t="s">
         <v>162</v>
       </c>
-      <c r="H10" s="267" t="s">
+      <c r="H10" s="161" t="s">
         <v>737</v>
       </c>
     </row>
@@ -4635,8 +4635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4664,35 +4664,35 @@
       <c r="G1" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="23.25">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
-      <c r="K3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="182"/>
     </row>
     <row r="4" spans="1:11" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
+      <c r="K4" s="183"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="90" t="s">
@@ -4706,52 +4706,52 @@
     </row>
     <row r="8" spans="1:11" ht="30.75" customHeight="1"/>
     <row r="9" spans="1:11">
-      <c r="A9" s="239" t="s">
+      <c r="A9" s="219" t="s">
         <v>482</v>
       </c>
-      <c r="B9" s="240"/>
-      <c r="C9" s="240"/>
-      <c r="D9" s="240"/>
-      <c r="E9" s="240"/>
-      <c r="F9" s="240"/>
-      <c r="G9" s="240"/>
-      <c r="H9" s="240"/>
-      <c r="I9" s="240"/>
-      <c r="J9" s="240"/>
-      <c r="K9" s="241"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="266" t="s">
+      <c r="B9" s="220"/>
+      <c r="C9" s="220"/>
+      <c r="D9" s="220"/>
+      <c r="E9" s="220"/>
+      <c r="F9" s="220"/>
+      <c r="G9" s="220"/>
+      <c r="H9" s="220"/>
+      <c r="I9" s="220"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="221"/>
+    </row>
+    <row r="10" spans="1:11" ht="32.25" customHeight="1">
+      <c r="A10" s="160" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="266" t="s">
+      <c r="B10" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="266" t="s">
+      <c r="C10" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="266" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="266" t="s">
+      <c r="D10" s="160" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="160" t="s">
         <v>812</v>
       </c>
-      <c r="F10" s="268" t="s">
+      <c r="F10" s="162" t="s">
         <v>140</v>
       </c>
-      <c r="G10" s="268" t="s">
+      <c r="G10" s="162" t="s">
         <v>141</v>
       </c>
-      <c r="H10" s="266" t="s">
+      <c r="H10" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="266" t="s">
+      <c r="I10" s="160" t="s">
         <v>169</v>
       </c>
-      <c r="J10" s="266" t="s">
+      <c r="J10" s="160" t="s">
         <v>162</v>
       </c>
-      <c r="K10" s="267" t="s">
+      <c r="K10" s="161" t="s">
         <v>737</v>
       </c>
     </row>
@@ -4841,8 +4841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4877,16 +4877,16 @@
       <c r="H3" s="153"/>
     </row>
     <row r="4" spans="1:8" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>474</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="90" t="s">
@@ -4900,40 +4900,40 @@
     </row>
     <row r="8" spans="1:8" ht="30.75" customHeight="1"/>
     <row r="9" spans="1:8">
-      <c r="A9" s="239" t="s">
+      <c r="A9" s="219" t="s">
         <v>482</v>
       </c>
-      <c r="B9" s="240"/>
-      <c r="C9" s="240"/>
-      <c r="D9" s="240"/>
-      <c r="E9" s="240"/>
-      <c r="F9" s="240"/>
-      <c r="G9" s="240"/>
-      <c r="H9" s="241"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A10" s="266" t="s">
+      <c r="B9" s="220"/>
+      <c r="C9" s="220"/>
+      <c r="D9" s="220"/>
+      <c r="E9" s="220"/>
+      <c r="F9" s="220"/>
+      <c r="G9" s="220"/>
+      <c r="H9" s="221"/>
+    </row>
+    <row r="10" spans="1:8" ht="30.75" customHeight="1">
+      <c r="A10" s="160" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="266" t="s">
+      <c r="B10" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="266" t="s">
+      <c r="C10" s="160" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="266" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="266" t="s">
+      <c r="D10" s="160" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="266" t="s">
+      <c r="F10" s="160" t="s">
         <v>169</v>
       </c>
-      <c r="G10" s="266" t="s">
+      <c r="G10" s="160" t="s">
         <v>162</v>
       </c>
-      <c r="H10" s="267" t="s">
+      <c r="H10" s="161" t="s">
         <v>737</v>
       </c>
     </row>
@@ -4986,7 +4986,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5021,44 +5021,44 @@
       <c r="F3" s="108"/>
     </row>
     <row r="4" spans="1:6" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>748</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A6" s="207" t="s">
+      <c r="A6" s="216" t="s">
         <v>747</v>
       </c>
-      <c r="B6" s="208"/>
-      <c r="C6" s="208"/>
-      <c r="D6" s="209"/>
-      <c r="E6" s="203" t="s">
+      <c r="B6" s="217"/>
+      <c r="C6" s="217"/>
+      <c r="D6" s="218"/>
+      <c r="E6" s="212" t="s">
         <v>573</v>
       </c>
-      <c r="F6" s="203" t="s">
+      <c r="F6" s="212" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="215" t="s">
         <v>387</v>
       </c>
-      <c r="B7" s="206"/>
-      <c r="C7" s="206" t="s">
+      <c r="B7" s="215"/>
+      <c r="C7" s="215" t="s">
         <v>388</v>
       </c>
-      <c r="D7" s="206"/>
-      <c r="E7" s="204"/>
-      <c r="F7" s="204"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
     </row>
     <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="77" t="s">
@@ -5073,8 +5073,8 @@
       <c r="D8" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="205"/>
-      <c r="F8" s="205"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
     </row>
     <row r="9" spans="1:6" s="48" customFormat="1" ht="38.25" customHeight="1">
       <c r="A9" s="120" t="str">
@@ -5179,63 +5179,63 @@
       <c r="A2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="23.25">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="182"/>
     </row>
     <row r="4" spans="1:12" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>467</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
+      <c r="K4" s="183"/>
+      <c r="L4" s="183"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1">
       <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="204" t="s">
         <v>475</v>
       </c>
-      <c r="B6" s="198"/>
+      <c r="B6" s="205"/>
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A7" s="211" t="s">
+      <c r="A7" s="242" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="212"/>
-      <c r="C7" s="200"/>
-      <c r="D7" s="200"/>
+      <c r="B7" s="243"/>
+      <c r="C7" s="206"/>
+      <c r="D7" s="206"/>
       <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A8" s="213" t="s">
+      <c r="A8" s="244" t="s">
         <v>194</v>
       </c>
-      <c r="B8" s="214"/>
-      <c r="C8" s="200"/>
-      <c r="D8" s="200"/>
+      <c r="B8" s="245"/>
+      <c r="C8" s="206"/>
+      <c r="D8" s="206"/>
       <c r="E8" s="63"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" customHeight="1">
@@ -5255,10 +5255,10 @@
       <c r="F10" s="88"/>
       <c r="G10" s="88"/>
       <c r="H10" s="88"/>
-      <c r="I10" s="233"/>
-      <c r="J10" s="233"/>
-      <c r="K10" s="233"/>
-      <c r="L10" s="233"/>
+      <c r="I10" s="234"/>
+      <c r="J10" s="234"/>
+      <c r="K10" s="234"/>
+      <c r="L10" s="234"/>
     </row>
     <row r="11" spans="1:12" ht="25.5" customHeight="1">
       <c r="A11" s="83" t="s">
@@ -5276,26 +5276,26 @@
       <c r="E11" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="F11" s="232"/>
-      <c r="G11" s="232"/>
-      <c r="H11" s="232"/>
-      <c r="I11" s="232"/>
-      <c r="J11" s="232"/>
-      <c r="K11" s="232"/>
-      <c r="L11" s="232"/>
+      <c r="F11" s="233"/>
+      <c r="G11" s="233"/>
+      <c r="H11" s="233"/>
+      <c r="I11" s="233"/>
+      <c r="J11" s="233"/>
+      <c r="K11" s="233"/>
+      <c r="L11" s="233"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1">
-      <c r="D12" s="216" t="s">
+      <c r="D12" s="239" t="s">
         <v>181</v>
       </c>
-      <c r="E12" s="217"/>
-      <c r="F12" s="217"/>
-      <c r="G12" s="217"/>
-      <c r="H12" s="217"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
-      <c r="K12" s="217"/>
-      <c r="L12" s="218"/>
+      <c r="E12" s="240"/>
+      <c r="F12" s="240"/>
+      <c r="G12" s="240"/>
+      <c r="H12" s="240"/>
+      <c r="I12" s="240"/>
+      <c r="J12" s="240"/>
+      <c r="K12" s="240"/>
+      <c r="L12" s="241"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1">
       <c r="D13" s="9" t="s">
@@ -5327,17 +5327,17 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1">
-      <c r="D14" s="216" t="s">
+      <c r="D14" s="239" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="217"/>
-      <c r="F14" s="217"/>
-      <c r="G14" s="217"/>
-      <c r="H14" s="217"/>
-      <c r="I14" s="217"/>
-      <c r="J14" s="217"/>
-      <c r="K14" s="217"/>
-      <c r="L14" s="218"/>
+      <c r="E14" s="240"/>
+      <c r="F14" s="240"/>
+      <c r="G14" s="240"/>
+      <c r="H14" s="240"/>
+      <c r="I14" s="240"/>
+      <c r="J14" s="240"/>
+      <c r="K14" s="240"/>
+      <c r="L14" s="241"/>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1">
       <c r="D15" s="9" t="s">
@@ -5349,40 +5349,40 @@
       <c r="F15" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G15" s="222"/>
-      <c r="H15" s="223"/>
-      <c r="I15" s="223"/>
-      <c r="J15" s="223"/>
-      <c r="K15" s="223"/>
-      <c r="L15" s="224"/>
+      <c r="G15" s="246"/>
+      <c r="H15" s="247"/>
+      <c r="I15" s="247"/>
+      <c r="J15" s="247"/>
+      <c r="K15" s="247"/>
+      <c r="L15" s="248"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1">
-      <c r="D16" s="216" t="s">
+      <c r="D16" s="239" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="217"/>
-      <c r="F16" s="217"/>
-      <c r="G16" s="217"/>
-      <c r="H16" s="217"/>
-      <c r="I16" s="217"/>
-      <c r="J16" s="217"/>
-      <c r="K16" s="217"/>
-      <c r="L16" s="218"/>
+      <c r="E16" s="240"/>
+      <c r="F16" s="240"/>
+      <c r="G16" s="240"/>
+      <c r="H16" s="240"/>
+      <c r="I16" s="240"/>
+      <c r="J16" s="240"/>
+      <c r="K16" s="240"/>
+      <c r="L16" s="241"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" customHeight="1">
       <c r="D17" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E17" s="235" t="s">
+      <c r="E17" s="236" t="s">
         <v>188</v>
       </c>
-      <c r="F17" s="236"/>
-      <c r="G17" s="236"/>
-      <c r="H17" s="236"/>
-      <c r="I17" s="236"/>
-      <c r="J17" s="236"/>
-      <c r="K17" s="236"/>
-      <c r="L17" s="237"/>
+      <c r="F17" s="237"/>
+      <c r="G17" s="237"/>
+      <c r="H17" s="237"/>
+      <c r="I17" s="237"/>
+      <c r="J17" s="237"/>
+      <c r="K17" s="237"/>
+      <c r="L17" s="238"/>
     </row>
     <row r="18" spans="1:13" ht="18.75" customHeight="1">
       <c r="A18" s="94" t="s">
@@ -5400,18 +5400,18 @@
       <c r="E18" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="219"/>
-      <c r="G18" s="220"/>
-      <c r="H18" s="220"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
-      <c r="K18" s="220"/>
-      <c r="L18" s="221"/>
+      <c r="F18" s="223"/>
+      <c r="G18" s="224"/>
+      <c r="H18" s="224"/>
+      <c r="I18" s="224"/>
+      <c r="J18" s="224"/>
+      <c r="K18" s="224"/>
+      <c r="L18" s="225"/>
     </row>
     <row r="19" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A19" s="227"/>
-      <c r="B19" s="227"/>
-      <c r="C19" s="215" t="s">
+      <c r="A19" s="228"/>
+      <c r="B19" s="228"/>
+      <c r="C19" s="222" t="s">
         <v>182</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -5444,9 +5444,9 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A20" s="234"/>
-      <c r="B20" s="234"/>
-      <c r="C20" s="215"/>
+      <c r="A20" s="235"/>
+      <c r="B20" s="235"/>
+      <c r="C20" s="222"/>
       <c r="D20" s="2" t="s">
         <v>119</v>
       </c>
@@ -5472,9 +5472,9 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A21" s="234"/>
-      <c r="B21" s="234"/>
-      <c r="C21" s="215"/>
+      <c r="A21" s="235"/>
+      <c r="B21" s="235"/>
+      <c r="C21" s="222"/>
       <c r="D21" s="2" t="s">
         <v>161</v>
       </c>
@@ -5498,9 +5498,9 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A22" s="234"/>
-      <c r="B22" s="234"/>
-      <c r="C22" s="215"/>
+      <c r="A22" s="235"/>
+      <c r="B22" s="235"/>
+      <c r="C22" s="222"/>
       <c r="D22" s="2" t="s">
         <v>193</v>
       </c>
@@ -5526,9 +5526,9 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A23" s="234"/>
-      <c r="B23" s="234"/>
-      <c r="C23" s="215" t="s">
+      <c r="A23" s="235"/>
+      <c r="B23" s="235"/>
+      <c r="C23" s="222" t="s">
         <v>183</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -5540,20 +5540,20 @@
       <c r="F23" s="24">
         <v>1</v>
       </c>
-      <c r="G23" s="215"/>
-      <c r="H23" s="215"/>
-      <c r="I23" s="215"/>
-      <c r="J23" s="215"/>
-      <c r="K23" s="215"/>
-      <c r="L23" s="215"/>
+      <c r="G23" s="222"/>
+      <c r="H23" s="222"/>
+      <c r="I23" s="222"/>
+      <c r="J23" s="222"/>
+      <c r="K23" s="222"/>
+      <c r="L23" s="222"/>
       <c r="M23" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A24" s="234"/>
-      <c r="B24" s="234"/>
-      <c r="C24" s="215"/>
+      <c r="A24" s="235"/>
+      <c r="B24" s="235"/>
+      <c r="C24" s="222"/>
       <c r="D24" s="2" t="s">
         <v>191</v>
       </c>
@@ -5563,17 +5563,17 @@
       <c r="F24" s="24">
         <v>1</v>
       </c>
-      <c r="G24" s="215"/>
-      <c r="H24" s="215"/>
-      <c r="I24" s="215"/>
-      <c r="J24" s="215"/>
-      <c r="K24" s="215"/>
-      <c r="L24" s="215"/>
+      <c r="G24" s="222"/>
+      <c r="H24" s="222"/>
+      <c r="I24" s="222"/>
+      <c r="J24" s="222"/>
+      <c r="K24" s="222"/>
+      <c r="L24" s="222"/>
     </row>
     <row r="25" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A25" s="234"/>
-      <c r="B25" s="234"/>
-      <c r="C25" s="215"/>
+      <c r="A25" s="235"/>
+      <c r="B25" s="235"/>
+      <c r="C25" s="222"/>
       <c r="D25" s="2" t="s">
         <v>192</v>
       </c>
@@ -5583,67 +5583,67 @@
       <c r="F25" s="24">
         <v>1</v>
       </c>
-      <c r="G25" s="215"/>
-      <c r="H25" s="215"/>
-      <c r="I25" s="215"/>
-      <c r="J25" s="215"/>
-      <c r="K25" s="215"/>
-      <c r="L25" s="215"/>
+      <c r="G25" s="222"/>
+      <c r="H25" s="222"/>
+      <c r="I25" s="222"/>
+      <c r="J25" s="222"/>
+      <c r="K25" s="222"/>
+      <c r="L25" s="222"/>
     </row>
     <row r="26" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A26" s="234"/>
-      <c r="B26" s="234"/>
-      <c r="C26" s="227" t="s">
+      <c r="A26" s="235"/>
+      <c r="B26" s="235"/>
+      <c r="C26" s="228" t="s">
         <v>186</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E26" s="229" t="s">
+      <c r="E26" s="230" t="s">
         <v>196</v>
       </c>
-      <c r="F26" s="230"/>
-      <c r="G26" s="230"/>
-      <c r="H26" s="230"/>
-      <c r="I26" s="230"/>
-      <c r="J26" s="230"/>
-      <c r="K26" s="230"/>
-      <c r="L26" s="231"/>
+      <c r="F26" s="231"/>
+      <c r="G26" s="231"/>
+      <c r="H26" s="231"/>
+      <c r="I26" s="231"/>
+      <c r="J26" s="231"/>
+      <c r="K26" s="231"/>
+      <c r="L26" s="232"/>
       <c r="M26" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A27" s="228"/>
-      <c r="B27" s="228"/>
-      <c r="C27" s="228"/>
+      <c r="A27" s="229"/>
+      <c r="B27" s="229"/>
+      <c r="C27" s="229"/>
       <c r="D27" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E27" s="229" t="s">
+      <c r="E27" s="230" t="s">
         <v>190</v>
       </c>
-      <c r="F27" s="230"/>
-      <c r="G27" s="230"/>
-      <c r="H27" s="230"/>
-      <c r="I27" s="230"/>
-      <c r="J27" s="230"/>
-      <c r="K27" s="230"/>
-      <c r="L27" s="231"/>
+      <c r="F27" s="231"/>
+      <c r="G27" s="231"/>
+      <c r="H27" s="231"/>
+      <c r="I27" s="231"/>
+      <c r="J27" s="231"/>
+      <c r="K27" s="231"/>
+      <c r="L27" s="232"/>
     </row>
     <row r="28" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A28" s="225"/>
-      <c r="B28" s="226"/>
-      <c r="C28" s="226"/>
-      <c r="D28" s="226"/>
-      <c r="E28" s="226"/>
-      <c r="F28" s="226"/>
-      <c r="G28" s="226"/>
-      <c r="H28" s="226"/>
-      <c r="I28" s="226"/>
-      <c r="J28" s="226"/>
-      <c r="K28" s="226"/>
-      <c r="L28" s="226"/>
+      <c r="A28" s="226"/>
+      <c r="B28" s="227"/>
+      <c r="C28" s="227"/>
+      <c r="D28" s="227"/>
+      <c r="E28" s="227"/>
+      <c r="F28" s="227"/>
+      <c r="G28" s="227"/>
+      <c r="H28" s="227"/>
+      <c r="I28" s="227"/>
+      <c r="J28" s="227"/>
+      <c r="K28" s="227"/>
+      <c r="L28" s="227"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" customHeight="1">
       <c r="A29" s="94" t="s">
@@ -5661,16 +5661,16 @@
       <c r="E29" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="219"/>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
-      <c r="I29" s="220"/>
-      <c r="J29" s="220"/>
-      <c r="K29" s="220"/>
-      <c r="L29" s="221"/>
+      <c r="F29" s="223"/>
+      <c r="G29" s="224"/>
+      <c r="H29" s="224"/>
+      <c r="I29" s="224"/>
+      <c r="J29" s="224"/>
+      <c r="K29" s="224"/>
+      <c r="L29" s="225"/>
     </row>
     <row r="30" spans="1:13" ht="18.75" customHeight="1">
-      <c r="C30" s="215" t="s">
+      <c r="C30" s="222" t="s">
         <v>182</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -5698,7 +5698,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="18.75" customHeight="1">
-      <c r="C31" s="215"/>
+      <c r="C31" s="222"/>
       <c r="D31" s="2" t="s">
         <v>119</v>
       </c>
@@ -5724,7 +5724,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="18.75" customHeight="1">
-      <c r="C32" s="215"/>
+      <c r="C32" s="222"/>
       <c r="D32" s="2" t="s">
         <v>161</v>
       </c>
@@ -5748,7 +5748,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C33" s="215"/>
+      <c r="C33" s="222"/>
       <c r="D33" s="2" t="s">
         <v>193</v>
       </c>
@@ -5787,16 +5787,16 @@
       <c r="E35" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="219"/>
-      <c r="G35" s="220"/>
-      <c r="H35" s="220"/>
-      <c r="I35" s="220"/>
-      <c r="J35" s="220"/>
-      <c r="K35" s="220"/>
-      <c r="L35" s="221"/>
+      <c r="F35" s="223"/>
+      <c r="G35" s="224"/>
+      <c r="H35" s="224"/>
+      <c r="I35" s="224"/>
+      <c r="J35" s="224"/>
+      <c r="K35" s="224"/>
+      <c r="L35" s="225"/>
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C36" s="215" t="s">
+      <c r="C36" s="222" t="s">
         <v>182</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -5824,7 +5824,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C37" s="215"/>
+      <c r="C37" s="222"/>
       <c r="D37" s="2" t="s">
         <v>119</v>
       </c>
@@ -5850,7 +5850,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C38" s="215"/>
+      <c r="C38" s="222"/>
       <c r="D38" s="2" t="s">
         <v>161</v>
       </c>
@@ -5874,7 +5874,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C39" s="215"/>
+      <c r="C39" s="222"/>
       <c r="D39" s="2" t="s">
         <v>193</v>
       </c>
@@ -5898,7 +5898,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C40" s="215" t="s">
+      <c r="C40" s="222" t="s">
         <v>183</v>
       </c>
       <c r="D40" s="2" t="s">
@@ -5910,15 +5910,15 @@
       <c r="F40" s="24">
         <v>1</v>
       </c>
-      <c r="G40" s="215"/>
-      <c r="H40" s="215"/>
-      <c r="I40" s="215"/>
-      <c r="J40" s="215"/>
-      <c r="K40" s="215"/>
-      <c r="L40" s="215"/>
+      <c r="G40" s="222"/>
+      <c r="H40" s="222"/>
+      <c r="I40" s="222"/>
+      <c r="J40" s="222"/>
+      <c r="K40" s="222"/>
+      <c r="L40" s="222"/>
     </row>
     <row r="41" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C41" s="215"/>
+      <c r="C41" s="222"/>
       <c r="D41" s="2" t="s">
         <v>191</v>
       </c>
@@ -5928,15 +5928,15 @@
       <c r="F41" s="24">
         <v>1</v>
       </c>
-      <c r="G41" s="215"/>
-      <c r="H41" s="215"/>
-      <c r="I41" s="215"/>
-      <c r="J41" s="215"/>
-      <c r="K41" s="215"/>
-      <c r="L41" s="215"/>
+      <c r="G41" s="222"/>
+      <c r="H41" s="222"/>
+      <c r="I41" s="222"/>
+      <c r="J41" s="222"/>
+      <c r="K41" s="222"/>
+      <c r="L41" s="222"/>
     </row>
     <row r="42" spans="1:12" ht="18.75" customHeight="1">
-      <c r="C42" s="215"/>
+      <c r="C42" s="222"/>
       <c r="D42" s="2" t="s">
         <v>200</v>
       </c>
@@ -5946,16 +5946,33 @@
       <c r="F42" s="24">
         <v>1</v>
       </c>
-      <c r="G42" s="215"/>
-      <c r="H42" s="215"/>
-      <c r="I42" s="215"/>
-      <c r="J42" s="215"/>
-      <c r="K42" s="215"/>
-      <c r="L42" s="215"/>
+      <c r="G42" s="222"/>
+      <c r="H42" s="222"/>
+      <c r="I42" s="222"/>
+      <c r="J42" s="222"/>
+      <c r="K42" s="222"/>
+      <c r="L42" s="222"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="33">
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="G40:L40"/>
+    <mergeCell ref="G41:L41"/>
+    <mergeCell ref="G42:L42"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="F29:L29"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="G23:L23"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D16:L16"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="G24:L24"/>
     <mergeCell ref="A3:L3"/>
@@ -5972,23 +5989,6 @@
     <mergeCell ref="E17:L17"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="D14:L14"/>
-    <mergeCell ref="G23:L23"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D16:L16"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="G40:L40"/>
-    <mergeCell ref="G41:L41"/>
-    <mergeCell ref="G42:L42"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="F29:L29"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="G15:L15"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19:G22 G30:G33 G36:G39">
@@ -6070,23 +6070,23 @@
       <c r="A6" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="238"/>
+      <c r="E6" s="249"/>
     </row>
     <row r="7" spans="1:9" s="91" customFormat="1" ht="14.25" customHeight="1">
       <c r="A7" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="238"/>
+      <c r="E7" s="249"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="242" t="s">
+      <c r="A9" s="250" t="s">
         <v>482</v>
       </c>
-      <c r="B9" s="242"/>
-      <c r="C9" s="242"/>
-      <c r="D9" s="242"/>
-      <c r="E9" s="242"/>
-      <c r="F9" s="242"/>
+      <c r="B9" s="250"/>
+      <c r="C9" s="250"/>
+      <c r="D9" s="250"/>
+      <c r="E9" s="250"/>
+      <c r="F9" s="250"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
       <c r="A10" s="7" t="s">
@@ -6171,14 +6171,14 @@
       <c r="F14" s="80"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="239" t="s">
+      <c r="A15" s="219" t="s">
         <v>486</v>
       </c>
-      <c r="B15" s="240"/>
-      <c r="C15" s="240"/>
-      <c r="D15" s="240"/>
-      <c r="E15" s="240"/>
-      <c r="F15" s="241"/>
+      <c r="B15" s="220"/>
+      <c r="C15" s="220"/>
+      <c r="D15" s="220"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="221"/>
     </row>
     <row r="16" spans="1:9" ht="15.75">
       <c r="A16" s="7" t="s">
@@ -6311,25 +6311,25 @@
       <c r="Q3" s="70"/>
     </row>
     <row r="4" spans="1:18" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>469</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
-      <c r="M4" s="176"/>
-      <c r="N4" s="176"/>
-      <c r="O4" s="176"/>
-      <c r="P4" s="176"/>
-      <c r="Q4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
+      <c r="K4" s="183"/>
+      <c r="L4" s="183"/>
+      <c r="M4" s="183"/>
+      <c r="N4" s="183"/>
+      <c r="O4" s="183"/>
+      <c r="P4" s="183"/>
+      <c r="Q4" s="183"/>
     </row>
     <row r="5" spans="1:18" ht="21" customHeight="1"/>
     <row r="6" spans="1:18">
@@ -6343,76 +6343,76 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A9" s="250" t="s">
+      <c r="A9" s="257" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="251"/>
-      <c r="C9" s="251"/>
-      <c r="D9" s="251"/>
-      <c r="E9" s="251"/>
-      <c r="F9" s="251"/>
-      <c r="G9" s="251"/>
-      <c r="H9" s="251"/>
-      <c r="I9" s="251"/>
-      <c r="J9" s="251"/>
-      <c r="K9" s="251"/>
-      <c r="L9" s="251"/>
-      <c r="M9" s="251"/>
-      <c r="N9" s="251"/>
-      <c r="O9" s="251"/>
-      <c r="P9" s="251"/>
-      <c r="Q9" s="251"/>
-      <c r="R9" s="252"/>
+      <c r="B9" s="258"/>
+      <c r="C9" s="258"/>
+      <c r="D9" s="258"/>
+      <c r="E9" s="258"/>
+      <c r="F9" s="258"/>
+      <c r="G9" s="258"/>
+      <c r="H9" s="258"/>
+      <c r="I9" s="258"/>
+      <c r="J9" s="258"/>
+      <c r="K9" s="258"/>
+      <c r="L9" s="258"/>
+      <c r="M9" s="258"/>
+      <c r="N9" s="258"/>
+      <c r="O9" s="258"/>
+      <c r="P9" s="258"/>
+      <c r="Q9" s="258"/>
+      <c r="R9" s="259"/>
     </row>
     <row r="10" spans="1:18" ht="33" customHeight="1">
-      <c r="A10" s="244" t="s">
+      <c r="A10" s="255" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="244" t="s">
+      <c r="B10" s="255" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="244" t="s">
+      <c r="C10" s="255" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="244" t="s">
+      <c r="D10" s="255" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="248" t="s">
+      <c r="E10" s="252" t="s">
         <v>208</v>
       </c>
       <c r="F10" s="253"/>
-      <c r="G10" s="249"/>
-      <c r="H10" s="244" t="s">
+      <c r="G10" s="254"/>
+      <c r="H10" s="255" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="246" t="s">
+      <c r="I10" s="261" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="247"/>
-      <c r="K10" s="248" t="s">
+      <c r="J10" s="262"/>
+      <c r="K10" s="252" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="249"/>
-      <c r="M10" s="248" t="s">
+      <c r="L10" s="254"/>
+      <c r="M10" s="252" t="s">
         <v>213</v>
       </c>
-      <c r="N10" s="249"/>
+      <c r="N10" s="254"/>
       <c r="O10" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="P10" s="243" t="s">
+      <c r="P10" s="251" t="s">
         <v>214</v>
       </c>
-      <c r="Q10" s="243"/>
-      <c r="R10" s="210" t="s">
+      <c r="Q10" s="251"/>
+      <c r="R10" s="260" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="33" customHeight="1">
-      <c r="A11" s="245"/>
-      <c r="B11" s="245"/>
-      <c r="C11" s="245"/>
-      <c r="D11" s="245"/>
+      <c r="A11" s="256"/>
+      <c r="B11" s="256"/>
+      <c r="C11" s="256"/>
+      <c r="D11" s="256"/>
       <c r="E11" s="101" t="s">
         <v>205</v>
       </c>
@@ -6422,7 +6422,7 @@
       <c r="G11" s="101" t="s">
         <v>207</v>
       </c>
-      <c r="H11" s="245"/>
+      <c r="H11" s="256"/>
       <c r="I11" s="99" t="s">
         <v>135</v>
       </c>
@@ -6448,7 +6448,7 @@
       <c r="Q11" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="210"/>
+      <c r="R11" s="260"/>
     </row>
     <row r="12" spans="1:18" ht="107.25" customHeight="1">
       <c r="A12" s="59" t="s">
@@ -6557,76 +6557,76 @@
       <c r="R14" s="75"/>
     </row>
     <row r="15" spans="1:18" ht="18" customHeight="1">
-      <c r="A15" s="250" t="s">
+      <c r="A15" s="257" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="251"/>
-      <c r="C15" s="251"/>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
-      <c r="F15" s="251"/>
-      <c r="G15" s="251"/>
-      <c r="H15" s="251"/>
-      <c r="I15" s="251"/>
-      <c r="J15" s="251"/>
-      <c r="K15" s="251"/>
-      <c r="L15" s="251"/>
-      <c r="M15" s="251"/>
-      <c r="N15" s="251"/>
-      <c r="O15" s="251"/>
-      <c r="P15" s="251"/>
-      <c r="Q15" s="251"/>
-      <c r="R15" s="252"/>
+      <c r="B15" s="258"/>
+      <c r="C15" s="258"/>
+      <c r="D15" s="258"/>
+      <c r="E15" s="258"/>
+      <c r="F15" s="258"/>
+      <c r="G15" s="258"/>
+      <c r="H15" s="258"/>
+      <c r="I15" s="258"/>
+      <c r="J15" s="258"/>
+      <c r="K15" s="258"/>
+      <c r="L15" s="258"/>
+      <c r="M15" s="258"/>
+      <c r="N15" s="258"/>
+      <c r="O15" s="258"/>
+      <c r="P15" s="258"/>
+      <c r="Q15" s="258"/>
+      <c r="R15" s="259"/>
     </row>
     <row r="16" spans="1:18" ht="33" customHeight="1">
-      <c r="A16" s="244" t="s">
+      <c r="A16" s="255" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="244" t="s">
+      <c r="B16" s="255" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="244" t="s">
+      <c r="C16" s="255" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="244" t="s">
+      <c r="D16" s="255" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="248" t="s">
+      <c r="E16" s="252" t="s">
         <v>208</v>
       </c>
       <c r="F16" s="253"/>
-      <c r="G16" s="249"/>
-      <c r="H16" s="244" t="s">
+      <c r="G16" s="254"/>
+      <c r="H16" s="255" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="246" t="s">
+      <c r="I16" s="261" t="s">
         <v>211</v>
       </c>
-      <c r="J16" s="247"/>
-      <c r="K16" s="248" t="s">
+      <c r="J16" s="262"/>
+      <c r="K16" s="252" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="249"/>
-      <c r="M16" s="248" t="s">
+      <c r="L16" s="254"/>
+      <c r="M16" s="252" t="s">
         <v>213</v>
       </c>
-      <c r="N16" s="249"/>
+      <c r="N16" s="254"/>
       <c r="O16" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="P16" s="243" t="s">
+      <c r="P16" s="251" t="s">
         <v>214</v>
       </c>
-      <c r="Q16" s="243"/>
-      <c r="R16" s="210" t="s">
+      <c r="Q16" s="251"/>
+      <c r="R16" s="260" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="33" customHeight="1">
-      <c r="A17" s="245"/>
-      <c r="B17" s="245"/>
-      <c r="C17" s="245"/>
-      <c r="D17" s="245"/>
+      <c r="A17" s="256"/>
+      <c r="B17" s="256"/>
+      <c r="C17" s="256"/>
+      <c r="D17" s="256"/>
       <c r="E17" s="101" t="s">
         <v>205</v>
       </c>
@@ -6636,7 +6636,7 @@
       <c r="G17" s="101" t="s">
         <v>207</v>
       </c>
-      <c r="H17" s="245"/>
+      <c r="H17" s="256"/>
       <c r="I17" s="99" t="s">
         <v>135</v>
       </c>
@@ -6662,7 +6662,7 @@
       <c r="Q17" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="R17" s="210"/>
+      <c r="R17" s="260"/>
     </row>
     <row r="18" spans="1:18" ht="21" customHeight="1">
       <c r="A18" s="59" t="s">
@@ -6754,16 +6754,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A4:Q4"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A9:R9"/>
-    <mergeCell ref="R10:R11"/>
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="C10:C11"/>
@@ -6779,6 +6769,16 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="H16:H17"/>
+    <mergeCell ref="A4:Q4"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A9:R9"/>
+    <mergeCell ref="R10:R11"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:L14 K18:L21">
@@ -6832,33 +6832,33 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.25">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
     </row>
     <row r="4" spans="1:10" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>470</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="37" t="s">
@@ -6877,33 +6877,33 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A10" s="257" t="s">
+      <c r="A10" s="266" t="s">
         <v>522</v>
       </c>
-      <c r="B10" s="257"/>
-      <c r="C10" s="257"/>
-      <c r="D10" s="257"/>
-      <c r="E10" s="257"/>
-      <c r="F10" s="257"/>
-      <c r="G10" s="257"/>
-      <c r="H10" s="257"/>
-      <c r="I10" s="257"/>
+      <c r="B10" s="266"/>
+      <c r="C10" s="266"/>
+      <c r="D10" s="266"/>
+      <c r="E10" s="266"/>
+      <c r="F10" s="266"/>
+      <c r="G10" s="266"/>
+      <c r="H10" s="266"/>
+      <c r="I10" s="266"/>
       <c r="J10" s="64"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A11" s="258" t="s">
+      <c r="A11" s="267" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="258"/>
-      <c r="C11" s="258"/>
-      <c r="D11" s="259" t="s">
+      <c r="B11" s="267"/>
+      <c r="C11" s="267"/>
+      <c r="D11" s="268" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="259"/>
-      <c r="F11" s="259"/>
-      <c r="G11" s="259"/>
-      <c r="H11" s="259"/>
-      <c r="I11" s="259"/>
+      <c r="E11" s="268"/>
+      <c r="F11" s="268"/>
+      <c r="G11" s="268"/>
+      <c r="H11" s="268"/>
+      <c r="I11" s="268"/>
       <c r="J11" s="65"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
@@ -6971,9 +6971,9 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A14" s="254"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="256"/>
+      <c r="A14" s="263"/>
+      <c r="B14" s="264"/>
+      <c r="C14" s="265"/>
       <c r="D14" s="13">
         <v>2</v>
       </c>
@@ -7051,9 +7051,9 @@
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A17" s="254"/>
-      <c r="B17" s="255"/>
-      <c r="C17" s="256"/>
+      <c r="A17" s="263"/>
+      <c r="B17" s="264"/>
+      <c r="C17" s="265"/>
       <c r="D17" s="13" t="s">
         <v>90</v>
       </c>
@@ -7124,33 +7124,33 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.25">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
     </row>
     <row r="4" spans="1:10" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>472</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="37" t="s">
@@ -7169,33 +7169,33 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1"/>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A10" s="257" t="s">
+      <c r="A10" s="266" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="257"/>
-      <c r="C10" s="257"/>
-      <c r="D10" s="257"/>
-      <c r="E10" s="257"/>
-      <c r="F10" s="257"/>
-      <c r="G10" s="257"/>
-      <c r="H10" s="257"/>
-      <c r="I10" s="257"/>
+      <c r="B10" s="266"/>
+      <c r="C10" s="266"/>
+      <c r="D10" s="266"/>
+      <c r="E10" s="266"/>
+      <c r="F10" s="266"/>
+      <c r="G10" s="266"/>
+      <c r="H10" s="266"/>
+      <c r="I10" s="266"/>
       <c r="J10" s="64"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A11" s="258" t="s">
+      <c r="A11" s="267" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="258"/>
-      <c r="C11" s="258"/>
-      <c r="D11" s="259" t="s">
+      <c r="B11" s="267"/>
+      <c r="C11" s="267"/>
+      <c r="D11" s="268" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="259"/>
-      <c r="F11" s="259"/>
-      <c r="G11" s="259"/>
-      <c r="H11" s="259"/>
-      <c r="I11" s="259"/>
+      <c r="E11" s="268"/>
+      <c r="F11" s="268"/>
+      <c r="G11" s="268"/>
+      <c r="H11" s="268"/>
+      <c r="I11" s="268"/>
       <c r="J11" s="65"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
@@ -7263,9 +7263,9 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A14" s="254"/>
-      <c r="B14" s="255"/>
-      <c r="C14" s="256"/>
+      <c r="A14" s="263"/>
+      <c r="B14" s="264"/>
+      <c r="C14" s="265"/>
       <c r="D14" s="13">
         <v>2</v>
       </c>
@@ -7343,9 +7343,9 @@
       <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A17" s="254"/>
-      <c r="B17" s="255"/>
-      <c r="C17" s="256"/>
+      <c r="A17" s="263"/>
+      <c r="B17" s="264"/>
+      <c r="C17" s="265"/>
       <c r="D17" s="13" t="s">
         <v>90</v>
       </c>
@@ -7421,12 +7421,12 @@
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
       <c r="B3" s="47"/>
-      <c r="C3" s="160" t="s">
+      <c r="C3" s="167" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="162"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="169"/>
       <c r="H3" s="2" t="s">
         <v>357</v>
       </c>
@@ -7442,10 +7442,10 @@
         <v>91</v>
       </c>
       <c r="B4" s="72"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="165"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="172"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17" t="s">
@@ -7951,17 +7951,17 @@
       <c r="A41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="158"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="159"/>
-      <c r="H41" s="159"/>
-      <c r="I41" s="159"/>
-      <c r="J41" s="159"/>
-      <c r="K41" s="159"/>
-      <c r="L41" s="159"/>
+      <c r="B41" s="165"/>
+      <c r="C41" s="166"/>
+      <c r="D41" s="166"/>
+      <c r="E41" s="166"/>
+      <c r="F41" s="166"/>
+      <c r="G41" s="166"/>
+      <c r="H41" s="166"/>
+      <c r="I41" s="166"/>
+      <c r="J41" s="166"/>
+      <c r="K41" s="166"/>
+      <c r="L41" s="166"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="5" t="s">
@@ -8065,14 +8065,14 @@
       <c r="A49" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="170"/>
-      <c r="C49" s="171"/>
-      <c r="D49" s="171"/>
-      <c r="E49" s="171"/>
-      <c r="F49" s="171"/>
-      <c r="G49" s="171"/>
-      <c r="H49" s="171"/>
-      <c r="I49" s="171"/>
+      <c r="B49" s="177"/>
+      <c r="C49" s="178"/>
+      <c r="D49" s="178"/>
+      <c r="E49" s="178"/>
+      <c r="F49" s="178"/>
+      <c r="G49" s="178"/>
+      <c r="H49" s="178"/>
+      <c r="I49" s="178"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="5" t="s">
@@ -8120,12 +8120,12 @@
       <c r="A54" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="156"/>
-      <c r="C54" s="157"/>
-      <c r="D54" s="157"/>
-      <c r="E54" s="157"/>
-      <c r="F54" s="157"/>
-      <c r="G54" s="157"/>
+      <c r="B54" s="163"/>
+      <c r="C54" s="164"/>
+      <c r="D54" s="164"/>
+      <c r="E54" s="164"/>
+      <c r="F54" s="164"/>
+      <c r="G54" s="164"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="50" t="s">
@@ -8154,10 +8154,10 @@
       <c r="A57" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B57" s="158"/>
-      <c r="C57" s="159"/>
-      <c r="D57" s="159"/>
-      <c r="E57" s="169"/>
+      <c r="B57" s="165"/>
+      <c r="C57" s="166"/>
+      <c r="D57" s="166"/>
+      <c r="E57" s="176"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="50" t="s">
@@ -8200,13 +8200,13 @@
       </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="166" t="s">
+      <c r="A62" s="173" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="167"/>
-      <c r="C62" s="167"/>
-      <c r="D62" s="167"/>
-      <c r="E62" s="168"/>
+      <c r="B62" s="174"/>
+      <c r="C62" s="174"/>
+      <c r="D62" s="174"/>
+      <c r="E62" s="175"/>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="2"/>
@@ -8263,13 +8263,13 @@
       <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:15">
-      <c r="A67" s="166" t="s">
+      <c r="A67" s="173" t="s">
         <v>24</v>
       </c>
-      <c r="B67" s="167"/>
-      <c r="C67" s="167"/>
-      <c r="D67" s="167"/>
-      <c r="E67" s="168"/>
+      <c r="B67" s="174"/>
+      <c r="C67" s="174"/>
+      <c r="D67" s="174"/>
+      <c r="E67" s="175"/>
     </row>
     <row r="68" spans="1:15">
       <c r="A68" s="2" t="s">
@@ -8425,7 +8425,7 @@
       <c r="M77" s="22" t="s">
         <v>441</v>
       </c>
-      <c r="N77" s="265"/>
+      <c r="N77" s="159"/>
     </row>
     <row r="78" spans="1:15">
       <c r="A78" s="21" t="s">
@@ -8452,13 +8452,13 @@
       <c r="H78" s="22" t="s">
         <v>441</v>
       </c>
-      <c r="I78" s="262"/>
-      <c r="J78" s="263"/>
-      <c r="K78" s="263"/>
-      <c r="L78" s="263"/>
-      <c r="M78" s="263"/>
-      <c r="N78" s="263"/>
-      <c r="O78" s="264"/>
+      <c r="I78" s="156"/>
+      <c r="J78" s="157"/>
+      <c r="K78" s="157"/>
+      <c r="L78" s="157"/>
+      <c r="M78" s="157"/>
+      <c r="N78" s="157"/>
+      <c r="O78" s="158"/>
     </row>
     <row r="79" spans="1:15">
       <c r="A79" s="19" t="s">
@@ -8597,37 +8597,37 @@
       <c r="A2" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="175"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="182"/>
     </row>
     <row r="4" spans="1:12" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>436</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
+      <c r="K4" s="183"/>
+      <c r="L4" s="183"/>
     </row>
     <row r="5" spans="1:12" ht="43.5" customHeight="1">
       <c r="A5" s="40"/>
@@ -8637,23 +8637,23 @@
       <c r="H5" s="126"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
-      <c r="A6" s="180"/>
-      <c r="B6" s="181"/>
-      <c r="C6" s="181"/>
-      <c r="D6" s="182"/>
-      <c r="E6" s="174" t="s">
+      <c r="A6" s="187"/>
+      <c r="B6" s="188"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="181" t="s">
         <v>453</v>
       </c>
-      <c r="F6" s="174"/>
-      <c r="G6" s="174" t="s">
+      <c r="F6" s="181"/>
+      <c r="G6" s="181" t="s">
         <v>456</v>
       </c>
-      <c r="H6" s="174"/>
-      <c r="I6" s="179" t="s">
+      <c r="H6" s="181"/>
+      <c r="I6" s="186" t="s">
         <v>457</v>
       </c>
-      <c r="J6" s="179"/>
-      <c r="K6" s="179"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="186"/>
       <c r="L6" s="154"/>
     </row>
     <row r="7" spans="1:12" ht="31.5">
@@ -8732,69 +8732,69 @@
     </row>
     <row r="9" spans="1:12" ht="46.5" customHeight="1"/>
     <row r="10" spans="1:12" ht="21" customHeight="1">
-      <c r="A10" s="177" t="s">
+      <c r="A10" s="184" t="s">
         <v>524</v>
       </c>
-      <c r="B10" s="178"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="178"/>
-      <c r="E10" s="178"/>
-      <c r="F10" s="178"/>
-      <c r="G10" s="178"/>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="178"/>
-      <c r="K10" s="178"/>
-      <c r="L10" s="178"/>
+      <c r="B10" s="185"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="185"/>
+      <c r="I10" s="185"/>
+      <c r="J10" s="185"/>
+      <c r="K10" s="185"/>
+      <c r="L10" s="185"/>
     </row>
     <row r="11" spans="1:12" ht="94.5" customHeight="1">
-      <c r="A11" s="172" t="s">
+      <c r="A11" s="179" t="s">
         <v>526</v>
       </c>
-      <c r="B11" s="173"/>
-      <c r="C11" s="173"/>
-      <c r="D11" s="173"/>
-      <c r="E11" s="173"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="173"/>
-      <c r="H11" s="173"/>
-      <c r="I11" s="173"/>
-      <c r="J11" s="173"/>
-      <c r="K11" s="173"/>
-      <c r="L11" s="173"/>
+      <c r="B11" s="180"/>
+      <c r="C11" s="180"/>
+      <c r="D11" s="180"/>
+      <c r="E11" s="180"/>
+      <c r="F11" s="180"/>
+      <c r="G11" s="180"/>
+      <c r="H11" s="180"/>
+      <c r="I11" s="180"/>
+      <c r="J11" s="180"/>
+      <c r="K11" s="180"/>
+      <c r="L11" s="180"/>
     </row>
     <row r="12" spans="1:12" ht="21" customHeight="1"/>
     <row r="13" spans="1:12" ht="21" customHeight="1">
-      <c r="A13" s="177" t="s">
+      <c r="A13" s="184" t="s">
         <v>525</v>
       </c>
-      <c r="B13" s="178"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="178"/>
-      <c r="G13" s="178"/>
-      <c r="H13" s="178"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="178"/>
-      <c r="K13" s="178"/>
-      <c r="L13" s="178"/>
+      <c r="B13" s="185"/>
+      <c r="C13" s="185"/>
+      <c r="D13" s="185"/>
+      <c r="E13" s="185"/>
+      <c r="F13" s="185"/>
+      <c r="G13" s="185"/>
+      <c r="H13" s="185"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="185"/>
+      <c r="K13" s="185"/>
+      <c r="L13" s="185"/>
     </row>
     <row r="14" spans="1:12" ht="249.75" customHeight="1">
-      <c r="A14" s="172" t="s">
+      <c r="A14" s="179" t="s">
         <v>527</v>
       </c>
-      <c r="B14" s="173"/>
-      <c r="C14" s="173"/>
-      <c r="D14" s="173"/>
-      <c r="E14" s="173"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="173"/>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="173"/>
-      <c r="L14" s="173"/>
+      <c r="B14" s="180"/>
+      <c r="C14" s="180"/>
+      <c r="D14" s="180"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+      <c r="J14" s="180"/>
+      <c r="K14" s="180"/>
+      <c r="L14" s="180"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -8866,14 +8866,14 @@
       <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:6" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>463</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
     </row>
     <row r="5" spans="1:6" ht="47.25" customHeight="1">
       <c r="A5" s="40"/>
@@ -9184,14 +9184,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" customHeight="1">
-      <c r="A21" s="183" t="s">
+      <c r="A21" s="190" t="s">
         <v>383</v>
       </c>
-      <c r="B21" s="184"/>
-      <c r="C21" s="184"/>
-      <c r="D21" s="184"/>
-      <c r="E21" s="184"/>
-      <c r="F21" s="185"/>
+      <c r="B21" s="191"/>
+      <c r="C21" s="191"/>
+      <c r="D21" s="191"/>
+      <c r="E21" s="191"/>
+      <c r="F21" s="192"/>
     </row>
     <row r="22" spans="1:6" ht="45">
       <c r="A22" s="10" t="s">
@@ -9303,29 +9303,29 @@
       <c r="E3" s="108"/>
     </row>
     <row r="4" spans="1:5" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>750</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
     </row>
     <row r="5" spans="1:5" ht="34.5" customHeight="1">
       <c r="A5" s="40"/>
     </row>
     <row r="6" spans="1:5" ht="31.5" customHeight="1">
-      <c r="A6" s="188" t="s">
+      <c r="A6" s="195" t="s">
         <v>354</v>
       </c>
-      <c r="B6" s="189"/>
-      <c r="C6" s="186" t="s">
+      <c r="B6" s="196"/>
+      <c r="C6" s="193" t="s">
         <v>389</v>
       </c>
-      <c r="D6" s="186" t="s">
+      <c r="D6" s="193" t="s">
         <v>390</v>
       </c>
-      <c r="E6" s="186" t="s">
+      <c r="E6" s="193" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9336,9 +9336,9 @@
       <c r="B7" s="77" t="s">
         <v>388</v>
       </c>
-      <c r="C7" s="187"/>
-      <c r="D7" s="187"/>
-      <c r="E7" s="187"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
     </row>
     <row r="8" spans="1:5" s="48" customFormat="1" ht="38.25" customHeight="1">
       <c r="A8" s="118" t="str">
@@ -9532,29 +9532,29 @@
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="23.25">
-      <c r="A2" s="175" t="str">
+      <c r="A2" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="182"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
     </row>
     <row r="3" spans="1:8" ht="23.25">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="183" t="s">
         <v>464</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
     </row>
     <row r="4" spans="1:8" ht="45.75" customHeight="1"/>
     <row r="5" spans="1:8">
@@ -9584,16 +9584,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A6" s="190" t="s">
+      <c r="A6" s="197" t="s">
         <v>335</v>
       </c>
-      <c r="B6" s="191"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="191"/>
-      <c r="E6" s="191"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="191"/>
-      <c r="H6" s="191"/>
+      <c r="B6" s="198"/>
+      <c r="C6" s="198"/>
+      <c r="D6" s="198"/>
+      <c r="E6" s="198"/>
+      <c r="F6" s="198"/>
+      <c r="G6" s="198"/>
+      <c r="H6" s="198"/>
     </row>
     <row r="7" spans="1:8" ht="86.25" customHeight="1">
       <c r="A7" s="15" t="s">
@@ -9737,16 +9737,16 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A13" s="192" t="s">
+      <c r="A13" s="199" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="193"/>
-      <c r="C13" s="193"/>
-      <c r="D13" s="193"/>
-      <c r="E13" s="193"/>
-      <c r="F13" s="193"/>
-      <c r="G13" s="193"/>
-      <c r="H13" s="193"/>
+      <c r="B13" s="200"/>
+      <c r="C13" s="200"/>
+      <c r="D13" s="200"/>
+      <c r="E13" s="200"/>
+      <c r="F13" s="200"/>
+      <c r="G13" s="200"/>
+      <c r="H13" s="200"/>
     </row>
     <row r="14" spans="1:8" ht="60">
       <c r="A14" s="15" t="s">
@@ -10073,16 +10073,16 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A28" s="192" t="s">
+      <c r="A28" s="199" t="s">
         <v>340</v>
       </c>
-      <c r="B28" s="193"/>
-      <c r="C28" s="193"/>
-      <c r="D28" s="193"/>
-      <c r="E28" s="193"/>
-      <c r="F28" s="193"/>
-      <c r="G28" s="193"/>
-      <c r="H28" s="193"/>
+      <c r="B28" s="200"/>
+      <c r="C28" s="200"/>
+      <c r="D28" s="200"/>
+      <c r="E28" s="200"/>
+      <c r="F28" s="200"/>
+      <c r="G28" s="200"/>
+      <c r="H28" s="200"/>
     </row>
     <row r="29" spans="1:8" ht="45">
       <c r="A29" s="15" t="s">
@@ -10513,26 +10513,26 @@
     </row>
     <row r="2" spans="1:7" ht="10.5" customHeight="1"/>
     <row r="3" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
       <c r="G3" s="109"/>
     </row>
     <row r="4" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>465</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
       <c r="G4" s="110"/>
     </row>
     <row r="5" spans="1:7" ht="39" customHeight="1"/>
@@ -10560,14 +10560,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A7" s="192" t="s">
+      <c r="A7" s="199" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="193"/>
-      <c r="C7" s="193"/>
-      <c r="D7" s="193"/>
-      <c r="E7" s="193"/>
-      <c r="F7" s="194"/>
+      <c r="B7" s="200"/>
+      <c r="C7" s="200"/>
+      <c r="D7" s="200"/>
+      <c r="E7" s="200"/>
+      <c r="F7" s="201"/>
       <c r="G7" s="122"/>
     </row>
     <row r="8" spans="1:7" ht="30.75" customHeight="1">
@@ -10697,14 +10697,14 @@
       <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A14" s="192" t="s">
+      <c r="A14" s="199" t="s">
         <v>333</v>
       </c>
-      <c r="B14" s="193"/>
-      <c r="C14" s="193"/>
-      <c r="D14" s="193"/>
-      <c r="E14" s="193"/>
-      <c r="F14" s="194"/>
+      <c r="B14" s="200"/>
+      <c r="C14" s="200"/>
+      <c r="D14" s="200"/>
+      <c r="E14" s="200"/>
+      <c r="F14" s="201"/>
       <c r="G14" s="122"/>
     </row>
     <row r="15" spans="1:7" ht="22.5" customHeight="1">
@@ -10881,14 +10881,14 @@
       <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7" ht="29.25" customHeight="1">
-      <c r="A23" s="192" t="s">
+      <c r="A23" s="199" t="s">
         <v>334</v>
       </c>
-      <c r="B23" s="193"/>
-      <c r="C23" s="193"/>
-      <c r="D23" s="193"/>
-      <c r="E23" s="193"/>
-      <c r="F23" s="194"/>
+      <c r="B23" s="200"/>
+      <c r="C23" s="200"/>
+      <c r="D23" s="200"/>
+      <c r="E23" s="200"/>
+      <c r="F23" s="201"/>
       <c r="G23" s="122"/>
     </row>
     <row r="24" spans="1:7" ht="31.5" customHeight="1">
@@ -11098,60 +11098,60 @@
     </row>
     <row r="2" spans="1:14" ht="11.25" customHeight="1"/>
     <row r="3" spans="1:14" ht="29.25" customHeight="1">
-      <c r="A3" s="175" t="str">
+      <c r="A3" s="182" t="str">
         <f>index!A1</f>
         <v>Especificação de Requisitos do SIOP (Sistema Integrado de Operações) - CSSFAA</v>
       </c>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
     </row>
     <row r="4" spans="1:14" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>466</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1"/>
     <row r="6" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A6" s="197" t="s">
+      <c r="A6" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="198"/>
+      <c r="B6" s="205"/>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A7" s="201" t="s">
+      <c r="A7" s="207" t="s">
         <v>569</v>
       </c>
-      <c r="B7" s="201"/>
-      <c r="C7" s="200"/>
-      <c r="D7" s="200"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="206"/>
+      <c r="D7" s="206"/>
       <c r="E7" s="74"/>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A8" s="202" t="s">
+      <c r="A8" s="208" t="s">
         <v>570</v>
       </c>
-      <c r="B8" s="202"/>
-      <c r="C8" s="200"/>
-      <c r="D8" s="200"/>
+      <c r="B8" s="208"/>
+      <c r="C8" s="206"/>
+      <c r="D8" s="206"/>
       <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A9" s="196" t="s">
+      <c r="A9" s="209" t="s">
         <v>571</v>
       </c>
-      <c r="B9" s="196"/>
+      <c r="B9" s="209"/>
       <c r="C9" s="111"/>
       <c r="D9" s="111"/>
       <c r="E9" s="111"/>
@@ -11160,10 +11160,10 @@
       <c r="I10" s="66"/>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="204" t="s">
         <v>476</v>
       </c>
-      <c r="B11" s="198"/>
+      <c r="B11" s="205"/>
     </row>
     <row r="12" spans="1:14" ht="33.75" customHeight="1">
       <c r="A12" s="77" t="s">
@@ -11192,16 +11192,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A13" s="195" t="s">
+      <c r="A13" s="202" t="s">
         <v>577</v>
       </c>
-      <c r="B13" s="195"/>
-      <c r="C13" s="195"/>
-      <c r="D13" s="195"/>
-      <c r="E13" s="195"/>
-      <c r="F13" s="195"/>
-      <c r="G13" s="195"/>
-      <c r="H13" s="260"/>
+      <c r="B13" s="202"/>
+      <c r="C13" s="202"/>
+      <c r="D13" s="202"/>
+      <c r="E13" s="202"/>
+      <c r="F13" s="202"/>
+      <c r="G13" s="202"/>
+      <c r="H13" s="203"/>
     </row>
     <row r="14" spans="1:14" ht="50.25" customHeight="1">
       <c r="A14" s="144" t="s">
@@ -11613,16 +11613,16 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A29" s="195" t="s">
+      <c r="A29" s="202" t="s">
         <v>669</v>
       </c>
-      <c r="B29" s="195"/>
-      <c r="C29" s="195"/>
-      <c r="D29" s="195"/>
-      <c r="E29" s="195"/>
-      <c r="F29" s="195"/>
-      <c r="G29" s="195"/>
-      <c r="H29" s="260"/>
+      <c r="B29" s="202"/>
+      <c r="C29" s="202"/>
+      <c r="D29" s="202"/>
+      <c r="E29" s="202"/>
+      <c r="F29" s="202"/>
+      <c r="G29" s="202"/>
+      <c r="H29" s="203"/>
     </row>
     <row r="30" spans="1:14" ht="50.25" customHeight="1">
       <c r="A30" s="141" t="s">
@@ -11918,16 +11918,16 @@
       <c r="N39" s="23"/>
     </row>
     <row r="40" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A40" s="195" t="s">
+      <c r="A40" s="202" t="s">
         <v>659</v>
       </c>
-      <c r="B40" s="195"/>
-      <c r="C40" s="195"/>
-      <c r="D40" s="195"/>
-      <c r="E40" s="195"/>
-      <c r="F40" s="195"/>
-      <c r="G40" s="195"/>
-      <c r="H40" s="260"/>
+      <c r="B40" s="202"/>
+      <c r="C40" s="202"/>
+      <c r="D40" s="202"/>
+      <c r="E40" s="202"/>
+      <c r="F40" s="202"/>
+      <c r="G40" s="202"/>
+      <c r="H40" s="203"/>
     </row>
     <row r="41" spans="1:14" ht="50.25" customHeight="1">
       <c r="A41" s="144" t="s">
@@ -12552,16 +12552,16 @@
       <c r="N61" s="23"/>
     </row>
     <row r="62" spans="1:14" ht="50.25" customHeight="1">
-      <c r="A62" s="195" t="s">
+      <c r="A62" s="202" t="s">
         <v>368</v>
       </c>
-      <c r="B62" s="195"/>
-      <c r="C62" s="195"/>
-      <c r="D62" s="195"/>
-      <c r="E62" s="195"/>
-      <c r="F62" s="195"/>
-      <c r="G62" s="195"/>
-      <c r="H62" s="260"/>
+      <c r="B62" s="202"/>
+      <c r="C62" s="202"/>
+      <c r="D62" s="202"/>
+      <c r="E62" s="202"/>
+      <c r="F62" s="202"/>
+      <c r="G62" s="202"/>
+      <c r="H62" s="203"/>
     </row>
     <row r="63" spans="1:14" ht="50.25" customHeight="1">
       <c r="A63" s="144" t="s">
@@ -12855,16 +12855,16 @@
       <c r="N74" s="23"/>
     </row>
     <row r="75" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A75" s="199" t="s">
+      <c r="A75" s="210" t="s">
         <v>372</v>
       </c>
-      <c r="B75" s="199"/>
-      <c r="C75" s="199"/>
-      <c r="D75" s="199"/>
-      <c r="E75" s="199"/>
-      <c r="F75" s="199"/>
-      <c r="G75" s="199"/>
-      <c r="H75" s="261"/>
+      <c r="B75" s="210"/>
+      <c r="C75" s="210"/>
+      <c r="D75" s="210"/>
+      <c r="E75" s="210"/>
+      <c r="F75" s="210"/>
+      <c r="G75" s="210"/>
+      <c r="H75" s="211"/>
     </row>
     <row r="76" spans="1:14" ht="50.25" customHeight="1">
       <c r="A76" s="141" t="s">
@@ -13135,16 +13135,16 @@
       <c r="H86" s="14"/>
     </row>
     <row r="87" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A87" s="195" t="s">
+      <c r="A87" s="202" t="s">
         <v>371</v>
       </c>
-      <c r="B87" s="195"/>
-      <c r="C87" s="195"/>
-      <c r="D87" s="195"/>
-      <c r="E87" s="195"/>
-      <c r="F87" s="195"/>
-      <c r="G87" s="195"/>
-      <c r="H87" s="260"/>
+      <c r="B87" s="202"/>
+      <c r="C87" s="202"/>
+      <c r="D87" s="202"/>
+      <c r="E87" s="202"/>
+      <c r="F87" s="202"/>
+      <c r="G87" s="202"/>
+      <c r="H87" s="203"/>
     </row>
     <row r="88" spans="1:14" ht="50.25" customHeight="1">
       <c r="A88" s="141" t="s">
@@ -13214,10 +13214,10 @@
     </row>
     <row r="91" spans="1:14" ht="33" customHeight="1"/>
     <row r="92" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A92" s="197" t="s">
+      <c r="A92" s="204" t="s">
         <v>350</v>
       </c>
-      <c r="B92" s="198"/>
+      <c r="B92" s="205"/>
     </row>
     <row r="93" spans="1:14" ht="33.75" customHeight="1">
       <c r="A93" s="77" t="s">
@@ -13246,16 +13246,16 @@
       </c>
     </row>
     <row r="94" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A94" s="195" t="s">
+      <c r="A94" s="202" t="s">
         <v>577</v>
       </c>
-      <c r="B94" s="195"/>
-      <c r="C94" s="195"/>
-      <c r="D94" s="195"/>
-      <c r="E94" s="195"/>
-      <c r="F94" s="195"/>
-      <c r="G94" s="195"/>
-      <c r="H94" s="260"/>
+      <c r="B94" s="202"/>
+      <c r="C94" s="202"/>
+      <c r="D94" s="202"/>
+      <c r="E94" s="202"/>
+      <c r="F94" s="202"/>
+      <c r="G94" s="202"/>
+      <c r="H94" s="203"/>
     </row>
     <row r="95" spans="1:14" ht="50.25" customHeight="1">
       <c r="A95" s="144" t="s">
@@ -13336,10 +13336,10 @@
       <c r="N97" s="23"/>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="197" t="s">
+      <c r="A99" s="204" t="s">
         <v>476</v>
       </c>
-      <c r="B99" s="198"/>
+      <c r="B99" s="205"/>
     </row>
     <row r="100" spans="1:14" ht="47.25">
       <c r="A100" s="77" t="s">
@@ -13368,16 +13368,16 @@
       </c>
     </row>
     <row r="101" spans="1:14">
-      <c r="A101" s="195" t="s">
+      <c r="A101" s="202" t="s">
         <v>577</v>
       </c>
-      <c r="B101" s="195"/>
-      <c r="C101" s="195"/>
-      <c r="D101" s="195"/>
-      <c r="E101" s="195"/>
-      <c r="F101" s="195"/>
-      <c r="G101" s="195"/>
-      <c r="H101" s="260"/>
+      <c r="B101" s="202"/>
+      <c r="C101" s="202"/>
+      <c r="D101" s="202"/>
+      <c r="E101" s="202"/>
+      <c r="F101" s="202"/>
+      <c r="G101" s="202"/>
+      <c r="H101" s="203"/>
     </row>
     <row r="102" spans="1:14" ht="30">
       <c r="A102" s="144" t="s">
@@ -13474,13 +13474,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A87:H87"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
@@ -13492,6 +13485,13 @@
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="A62:H62"/>
     <mergeCell ref="A75:H75"/>
+    <mergeCell ref="A87:H87"/>
+    <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E95:E97 E63:E74 E41:E61 E76:E86 E88:E90 E30:E39 E14:E28 E102:E105">
@@ -13549,44 +13549,44 @@
       <c r="F3" s="108"/>
     </row>
     <row r="4" spans="1:6" ht="23.25">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>749</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A6" s="207" t="s">
+      <c r="A6" s="216" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="208"/>
-      <c r="C6" s="208"/>
-      <c r="D6" s="209"/>
-      <c r="E6" s="203" t="s">
+      <c r="B6" s="217"/>
+      <c r="C6" s="217"/>
+      <c r="D6" s="218"/>
+      <c r="E6" s="212" t="s">
         <v>573</v>
       </c>
-      <c r="F6" s="203" t="s">
+      <c r="F6" s="212" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="215" t="s">
         <v>387</v>
       </c>
-      <c r="B7" s="206"/>
-      <c r="C7" s="206" t="s">
+      <c r="B7" s="215"/>
+      <c r="C7" s="215" t="s">
         <v>388</v>
       </c>
-      <c r="D7" s="206"/>
-      <c r="E7" s="204"/>
-      <c r="F7" s="204"/>
+      <c r="D7" s="215"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="213"/>
     </row>
     <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="77" t="s">
@@ -13601,8 +13601,8 @@
       <c r="D8" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="205"/>
-      <c r="F8" s="205"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
     </row>
     <row r="9" spans="1:6" s="48" customFormat="1" ht="38.25" customHeight="1">
       <c r="A9" s="120" t="str">

</xml_diff>

<commit_message>
Fixes Requirements Relations sheet
</commit_message>
<xml_diff>
--- a/Templates/SIOP-RSLIL-v2.1.xlsx
+++ b/Templates/SIOP-RSLIL-v2.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="842" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="848">
   <si>
     <t>Id</t>
   </si>
@@ -2955,6 +2955,9 @@
   </si>
   <si>
     <t>Constraint</t>
+  </si>
+  <si>
+    <t>Requirement Relation</t>
   </si>
 </sst>
 </file>
@@ -3836,16 +3839,25 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3857,15 +3869,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3899,6 +3902,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3908,6 +3920,27 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3947,77 +3980,47 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4635,7 +4638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4842,7 +4845,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A9" sqref="A9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4983,15 +4986,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
@@ -5030,111 +5033,132 @@
       <c r="E4" s="183"/>
       <c r="F4" s="183"/>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-    </row>
-    <row r="6" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A6" s="216" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="90" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="92" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" customHeight="1">
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="219" t="s">
+        <v>482</v>
+      </c>
+      <c r="B9" s="220"/>
+      <c r="C9" s="220"/>
+      <c r="D9" s="220"/>
+      <c r="E9" s="220"/>
+      <c r="F9" s="221"/>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" customHeight="1">
+      <c r="A10" s="216" t="s">
         <v>747</v>
       </c>
-      <c r="B6" s="217"/>
-      <c r="C6" s="217"/>
-      <c r="D6" s="218"/>
-      <c r="E6" s="212" t="s">
+      <c r="B10" s="217"/>
+      <c r="C10" s="217"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="212" t="s">
         <v>573</v>
       </c>
-      <c r="F6" s="212" t="s">
+      <c r="F10" s="212" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75">
-      <c r="A7" s="215" t="s">
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="215" t="s">
         <v>387</v>
       </c>
-      <c r="B7" s="215"/>
-      <c r="C7" s="215" t="s">
+      <c r="B11" s="215"/>
+      <c r="C11" s="215" t="s">
         <v>388</v>
       </c>
-      <c r="D7" s="215"/>
-      <c r="E7" s="213"/>
-      <c r="F7" s="213"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75">
-      <c r="A8" s="77" t="s">
+      <c r="D11" s="215"/>
+      <c r="E11" s="213"/>
+      <c r="F11" s="213"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75">
+      <c r="A12" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B12" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="77" t="s">
+      <c r="C12" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="145" t="s">
+      <c r="D12" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="214"/>
-      <c r="F8" s="214"/>
-    </row>
-    <row r="9" spans="1:6" s="48" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A9" s="120" t="str">
+      <c r="E12" s="214"/>
+      <c r="F12" s="214"/>
+    </row>
+    <row r="13" spans="1:6" s="48" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A13" s="120" t="str">
         <f>reqs.functional!A11</f>
         <v>fr1</v>
       </c>
-      <c r="B9" s="120" t="str">
+      <c r="B13" s="120" t="str">
         <f>reqs.functional!B11</f>
         <v>Functional Requirement 1</v>
       </c>
-      <c r="C9" s="120" t="str">
+      <c r="C13" s="120" t="str">
         <f>reqs.quality!A11</f>
         <v>QR1</v>
       </c>
-      <c r="D9" s="120" t="str">
+      <c r="D13" s="120" t="str">
         <f>reqs.quality!B11</f>
         <v>YYY</v>
       </c>
-      <c r="E9" s="121" t="s">
+      <c r="E13" s="121" t="s">
         <v>796</v>
       </c>
-      <c r="F9" s="120" t="s">
+      <c r="F13" s="120" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="48" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A10" s="120" t="str">
+    <row r="14" spans="1:6" s="48" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A14" s="120" t="str">
         <f>reqs.quality!A11</f>
         <v>QR1</v>
       </c>
-      <c r="B10" s="120" t="str">
+      <c r="B14" s="120" t="str">
         <f>reqs.quality!B11</f>
         <v>YYY</v>
       </c>
-      <c r="C10" s="120" t="str">
+      <c r="C14" s="120" t="str">
         <f>reqs.quality!A12</f>
         <v>QR2</v>
       </c>
-      <c r="D10" s="120" t="str">
+      <c r="D14" s="120" t="str">
         <f>reqs.quality!B12</f>
         <v>ZZZ</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E14" s="121" t="s">
         <v>798</v>
       </c>
-      <c r="F10" s="120" t="s">
+      <c r="F14" s="120" t="s">
         <v>572</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E14">
       <formula1>GoalDependencyType</formula1>
     </dataValidation>
   </dataValidations>
@@ -5215,27 +5239,27 @@
       <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A6" s="204" t="s">
+      <c r="A6" s="202" t="s">
         <v>475</v>
       </c>
-      <c r="B6" s="205"/>
+      <c r="B6" s="203"/>
     </row>
     <row r="7" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A7" s="242" t="s">
+      <c r="A7" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="243"/>
-      <c r="C7" s="206"/>
-      <c r="D7" s="206"/>
+      <c r="B7" s="233"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
       <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A8" s="244" t="s">
+      <c r="A8" s="234" t="s">
         <v>194</v>
       </c>
-      <c r="B8" s="245"/>
-      <c r="C8" s="206"/>
-      <c r="D8" s="206"/>
+      <c r="B8" s="235"/>
+      <c r="C8" s="209"/>
+      <c r="D8" s="209"/>
       <c r="E8" s="63"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" customHeight="1">
@@ -5255,10 +5279,10 @@
       <c r="F10" s="88"/>
       <c r="G10" s="88"/>
       <c r="H10" s="88"/>
-      <c r="I10" s="234"/>
-      <c r="J10" s="234"/>
-      <c r="K10" s="234"/>
-      <c r="L10" s="234"/>
+      <c r="I10" s="244"/>
+      <c r="J10" s="244"/>
+      <c r="K10" s="244"/>
+      <c r="L10" s="244"/>
     </row>
     <row r="11" spans="1:12" ht="25.5" customHeight="1">
       <c r="A11" s="83" t="s">
@@ -5276,26 +5300,26 @@
       <c r="E11" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="F11" s="233"/>
-      <c r="G11" s="233"/>
-      <c r="H11" s="233"/>
-      <c r="I11" s="233"/>
-      <c r="J11" s="233"/>
-      <c r="K11" s="233"/>
-      <c r="L11" s="233"/>
+      <c r="F11" s="243"/>
+      <c r="G11" s="243"/>
+      <c r="H11" s="243"/>
+      <c r="I11" s="243"/>
+      <c r="J11" s="243"/>
+      <c r="K11" s="243"/>
+      <c r="L11" s="243"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1">
-      <c r="D12" s="239" t="s">
+      <c r="D12" s="223" t="s">
         <v>181</v>
       </c>
-      <c r="E12" s="240"/>
-      <c r="F12" s="240"/>
-      <c r="G12" s="240"/>
-      <c r="H12" s="240"/>
-      <c r="I12" s="240"/>
-      <c r="J12" s="240"/>
-      <c r="K12" s="240"/>
-      <c r="L12" s="241"/>
+      <c r="E12" s="224"/>
+      <c r="F12" s="224"/>
+      <c r="G12" s="224"/>
+      <c r="H12" s="224"/>
+      <c r="I12" s="224"/>
+      <c r="J12" s="224"/>
+      <c r="K12" s="224"/>
+      <c r="L12" s="225"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1">
       <c r="D13" s="9" t="s">
@@ -5327,17 +5351,17 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="18.75" customHeight="1">
-      <c r="D14" s="239" t="s">
+      <c r="D14" s="223" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="240"/>
-      <c r="F14" s="240"/>
-      <c r="G14" s="240"/>
-      <c r="H14" s="240"/>
-      <c r="I14" s="240"/>
-      <c r="J14" s="240"/>
-      <c r="K14" s="240"/>
-      <c r="L14" s="241"/>
+      <c r="E14" s="224"/>
+      <c r="F14" s="224"/>
+      <c r="G14" s="224"/>
+      <c r="H14" s="224"/>
+      <c r="I14" s="224"/>
+      <c r="J14" s="224"/>
+      <c r="K14" s="224"/>
+      <c r="L14" s="225"/>
     </row>
     <row r="15" spans="1:12" ht="18.75" customHeight="1">
       <c r="D15" s="9" t="s">
@@ -5349,40 +5373,40 @@
       <c r="F15" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G15" s="246"/>
-      <c r="H15" s="247"/>
-      <c r="I15" s="247"/>
-      <c r="J15" s="247"/>
-      <c r="K15" s="247"/>
-      <c r="L15" s="248"/>
+      <c r="G15" s="229"/>
+      <c r="H15" s="230"/>
+      <c r="I15" s="230"/>
+      <c r="J15" s="230"/>
+      <c r="K15" s="230"/>
+      <c r="L15" s="231"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" customHeight="1">
-      <c r="D16" s="239" t="s">
+      <c r="D16" s="223" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="240"/>
-      <c r="F16" s="240"/>
-      <c r="G16" s="240"/>
-      <c r="H16" s="240"/>
-      <c r="I16" s="240"/>
-      <c r="J16" s="240"/>
-      <c r="K16" s="240"/>
-      <c r="L16" s="241"/>
+      <c r="E16" s="224"/>
+      <c r="F16" s="224"/>
+      <c r="G16" s="224"/>
+      <c r="H16" s="224"/>
+      <c r="I16" s="224"/>
+      <c r="J16" s="224"/>
+      <c r="K16" s="224"/>
+      <c r="L16" s="225"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" customHeight="1">
       <c r="D17" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E17" s="236" t="s">
+      <c r="E17" s="246" t="s">
         <v>188</v>
       </c>
-      <c r="F17" s="237"/>
-      <c r="G17" s="237"/>
-      <c r="H17" s="237"/>
-      <c r="I17" s="237"/>
-      <c r="J17" s="237"/>
-      <c r="K17" s="237"/>
-      <c r="L17" s="238"/>
+      <c r="F17" s="247"/>
+      <c r="G17" s="247"/>
+      <c r="H17" s="247"/>
+      <c r="I17" s="247"/>
+      <c r="J17" s="247"/>
+      <c r="K17" s="247"/>
+      <c r="L17" s="248"/>
     </row>
     <row r="18" spans="1:13" ht="18.75" customHeight="1">
       <c r="A18" s="94" t="s">
@@ -5400,17 +5424,17 @@
       <c r="E18" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="223"/>
-      <c r="G18" s="224"/>
-      <c r="H18" s="224"/>
-      <c r="I18" s="224"/>
-      <c r="J18" s="224"/>
-      <c r="K18" s="224"/>
-      <c r="L18" s="225"/>
+      <c r="F18" s="226"/>
+      <c r="G18" s="227"/>
+      <c r="H18" s="227"/>
+      <c r="I18" s="227"/>
+      <c r="J18" s="227"/>
+      <c r="K18" s="227"/>
+      <c r="L18" s="228"/>
     </row>
     <row r="19" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A19" s="228"/>
-      <c r="B19" s="228"/>
+      <c r="A19" s="238"/>
+      <c r="B19" s="238"/>
       <c r="C19" s="222" t="s">
         <v>182</v>
       </c>
@@ -5444,8 +5468,8 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A20" s="235"/>
-      <c r="B20" s="235"/>
+      <c r="A20" s="245"/>
+      <c r="B20" s="245"/>
       <c r="C20" s="222"/>
       <c r="D20" s="2" t="s">
         <v>119</v>
@@ -5472,8 +5496,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A21" s="235"/>
-      <c r="B21" s="235"/>
+      <c r="A21" s="245"/>
+      <c r="B21" s="245"/>
       <c r="C21" s="222"/>
       <c r="D21" s="2" t="s">
         <v>161</v>
@@ -5498,8 +5522,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A22" s="235"/>
-      <c r="B22" s="235"/>
+      <c r="A22" s="245"/>
+      <c r="B22" s="245"/>
       <c r="C22" s="222"/>
       <c r="D22" s="2" t="s">
         <v>193</v>
@@ -5526,8 +5550,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A23" s="235"/>
-      <c r="B23" s="235"/>
+      <c r="A23" s="245"/>
+      <c r="B23" s="245"/>
       <c r="C23" s="222" t="s">
         <v>183</v>
       </c>
@@ -5551,8 +5575,8 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A24" s="235"/>
-      <c r="B24" s="235"/>
+      <c r="A24" s="245"/>
+      <c r="B24" s="245"/>
       <c r="C24" s="222"/>
       <c r="D24" s="2" t="s">
         <v>191</v>
@@ -5571,8 +5595,8 @@
       <c r="L24" s="222"/>
     </row>
     <row r="25" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A25" s="235"/>
-      <c r="B25" s="235"/>
+      <c r="A25" s="245"/>
+      <c r="B25" s="245"/>
       <c r="C25" s="222"/>
       <c r="D25" s="2" t="s">
         <v>192</v>
@@ -5591,59 +5615,59 @@
       <c r="L25" s="222"/>
     </row>
     <row r="26" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A26" s="235"/>
-      <c r="B26" s="235"/>
-      <c r="C26" s="228" t="s">
+      <c r="A26" s="245"/>
+      <c r="B26" s="245"/>
+      <c r="C26" s="238" t="s">
         <v>186</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E26" s="230" t="s">
+      <c r="E26" s="240" t="s">
         <v>196</v>
       </c>
-      <c r="F26" s="231"/>
-      <c r="G26" s="231"/>
-      <c r="H26" s="231"/>
-      <c r="I26" s="231"/>
-      <c r="J26" s="231"/>
-      <c r="K26" s="231"/>
-      <c r="L26" s="232"/>
+      <c r="F26" s="241"/>
+      <c r="G26" s="241"/>
+      <c r="H26" s="241"/>
+      <c r="I26" s="241"/>
+      <c r="J26" s="241"/>
+      <c r="K26" s="241"/>
+      <c r="L26" s="242"/>
       <c r="M26" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A27" s="229"/>
-      <c r="B27" s="229"/>
-      <c r="C27" s="229"/>
+      <c r="A27" s="239"/>
+      <c r="B27" s="239"/>
+      <c r="C27" s="239"/>
       <c r="D27" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E27" s="230" t="s">
+      <c r="E27" s="240" t="s">
         <v>190</v>
       </c>
-      <c r="F27" s="231"/>
-      <c r="G27" s="231"/>
-      <c r="H27" s="231"/>
-      <c r="I27" s="231"/>
-      <c r="J27" s="231"/>
-      <c r="K27" s="231"/>
-      <c r="L27" s="232"/>
+      <c r="F27" s="241"/>
+      <c r="G27" s="241"/>
+      <c r="H27" s="241"/>
+      <c r="I27" s="241"/>
+      <c r="J27" s="241"/>
+      <c r="K27" s="241"/>
+      <c r="L27" s="242"/>
     </row>
     <row r="28" spans="1:13" ht="22.5" customHeight="1">
-      <c r="A28" s="226"/>
-      <c r="B28" s="227"/>
-      <c r="C28" s="227"/>
-      <c r="D28" s="227"/>
-      <c r="E28" s="227"/>
-      <c r="F28" s="227"/>
-      <c r="G28" s="227"/>
-      <c r="H28" s="227"/>
-      <c r="I28" s="227"/>
-      <c r="J28" s="227"/>
-      <c r="K28" s="227"/>
-      <c r="L28" s="227"/>
+      <c r="A28" s="236"/>
+      <c r="B28" s="237"/>
+      <c r="C28" s="237"/>
+      <c r="D28" s="237"/>
+      <c r="E28" s="237"/>
+      <c r="F28" s="237"/>
+      <c r="G28" s="237"/>
+      <c r="H28" s="237"/>
+      <c r="I28" s="237"/>
+      <c r="J28" s="237"/>
+      <c r="K28" s="237"/>
+      <c r="L28" s="237"/>
     </row>
     <row r="29" spans="1:13" ht="18.75" customHeight="1">
       <c r="A29" s="94" t="s">
@@ -5661,13 +5685,13 @@
       <c r="E29" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="F29" s="223"/>
-      <c r="G29" s="224"/>
-      <c r="H29" s="224"/>
-      <c r="I29" s="224"/>
-      <c r="J29" s="224"/>
-      <c r="K29" s="224"/>
-      <c r="L29" s="225"/>
+      <c r="F29" s="226"/>
+      <c r="G29" s="227"/>
+      <c r="H29" s="227"/>
+      <c r="I29" s="227"/>
+      <c r="J29" s="227"/>
+      <c r="K29" s="227"/>
+      <c r="L29" s="228"/>
     </row>
     <row r="30" spans="1:13" ht="18.75" customHeight="1">
       <c r="C30" s="222" t="s">
@@ -5787,13 +5811,13 @@
       <c r="E35" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="223"/>
-      <c r="G35" s="224"/>
-      <c r="H35" s="224"/>
-      <c r="I35" s="224"/>
-      <c r="J35" s="224"/>
-      <c r="K35" s="224"/>
-      <c r="L35" s="225"/>
+      <c r="F35" s="226"/>
+      <c r="G35" s="227"/>
+      <c r="H35" s="227"/>
+      <c r="I35" s="227"/>
+      <c r="J35" s="227"/>
+      <c r="K35" s="227"/>
+      <c r="L35" s="228"/>
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1">
       <c r="C36" s="222" t="s">
@@ -5956,25 +5980,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="33">
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="G40:L40"/>
-    <mergeCell ref="G41:L41"/>
-    <mergeCell ref="G42:L42"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="F29:L29"/>
-    <mergeCell ref="F18:L18"/>
-    <mergeCell ref="G15:L15"/>
-    <mergeCell ref="G23:L23"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D16:L16"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G24:L24"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="F35:L35"/>
@@ -5989,6 +5994,25 @@
     <mergeCell ref="E17:L17"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="D14:L14"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D16:L16"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G24:L24"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="G40:L40"/>
+    <mergeCell ref="G41:L41"/>
+    <mergeCell ref="G42:L42"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="F29:L29"/>
+    <mergeCell ref="F18:L18"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="G23:L23"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19:G22 G30:G33 G36:G39">
@@ -6343,76 +6367,76 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A9" s="257" t="s">
+      <c r="A9" s="259" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="258"/>
-      <c r="C9" s="258"/>
-      <c r="D9" s="258"/>
-      <c r="E9" s="258"/>
-      <c r="F9" s="258"/>
-      <c r="G9" s="258"/>
-      <c r="H9" s="258"/>
-      <c r="I9" s="258"/>
-      <c r="J9" s="258"/>
-      <c r="K9" s="258"/>
-      <c r="L9" s="258"/>
-      <c r="M9" s="258"/>
-      <c r="N9" s="258"/>
-      <c r="O9" s="258"/>
-      <c r="P9" s="258"/>
-      <c r="Q9" s="258"/>
-      <c r="R9" s="259"/>
+      <c r="B9" s="260"/>
+      <c r="C9" s="260"/>
+      <c r="D9" s="260"/>
+      <c r="E9" s="260"/>
+      <c r="F9" s="260"/>
+      <c r="G9" s="260"/>
+      <c r="H9" s="260"/>
+      <c r="I9" s="260"/>
+      <c r="J9" s="260"/>
+      <c r="K9" s="260"/>
+      <c r="L9" s="260"/>
+      <c r="M9" s="260"/>
+      <c r="N9" s="260"/>
+      <c r="O9" s="260"/>
+      <c r="P9" s="260"/>
+      <c r="Q9" s="260"/>
+      <c r="R9" s="261"/>
     </row>
     <row r="10" spans="1:18" ht="33" customHeight="1">
-      <c r="A10" s="255" t="s">
+      <c r="A10" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="255" t="s">
+      <c r="B10" s="253" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="255" t="s">
+      <c r="C10" s="253" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="255" t="s">
+      <c r="D10" s="253" t="s">
         <v>164</v>
       </c>
-      <c r="E10" s="252" t="s">
+      <c r="E10" s="257" t="s">
         <v>208</v>
       </c>
-      <c r="F10" s="253"/>
-      <c r="G10" s="254"/>
-      <c r="H10" s="255" t="s">
+      <c r="F10" s="262"/>
+      <c r="G10" s="258"/>
+      <c r="H10" s="253" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="261" t="s">
+      <c r="I10" s="255" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="262"/>
-      <c r="K10" s="252" t="s">
+      <c r="J10" s="256"/>
+      <c r="K10" s="257" t="s">
         <v>74</v>
       </c>
-      <c r="L10" s="254"/>
-      <c r="M10" s="252" t="s">
+      <c r="L10" s="258"/>
+      <c r="M10" s="257" t="s">
         <v>213</v>
       </c>
-      <c r="N10" s="254"/>
+      <c r="N10" s="258"/>
       <c r="O10" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="P10" s="251" t="s">
+      <c r="P10" s="252" t="s">
         <v>214</v>
       </c>
-      <c r="Q10" s="251"/>
-      <c r="R10" s="260" t="s">
+      <c r="Q10" s="252"/>
+      <c r="R10" s="251" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="33" customHeight="1">
-      <c r="A11" s="256"/>
-      <c r="B11" s="256"/>
-      <c r="C11" s="256"/>
-      <c r="D11" s="256"/>
+      <c r="A11" s="254"/>
+      <c r="B11" s="254"/>
+      <c r="C11" s="254"/>
+      <c r="D11" s="254"/>
       <c r="E11" s="101" t="s">
         <v>205</v>
       </c>
@@ -6422,7 +6446,7 @@
       <c r="G11" s="101" t="s">
         <v>207</v>
       </c>
-      <c r="H11" s="256"/>
+      <c r="H11" s="254"/>
       <c r="I11" s="99" t="s">
         <v>135</v>
       </c>
@@ -6448,7 +6472,7 @@
       <c r="Q11" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="260"/>
+      <c r="R11" s="251"/>
     </row>
     <row r="12" spans="1:18" ht="107.25" customHeight="1">
       <c r="A12" s="59" t="s">
@@ -6557,76 +6581,76 @@
       <c r="R14" s="75"/>
     </row>
     <row r="15" spans="1:18" ht="18" customHeight="1">
-      <c r="A15" s="257" t="s">
+      <c r="A15" s="259" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="258"/>
-      <c r="C15" s="258"/>
-      <c r="D15" s="258"/>
-      <c r="E15" s="258"/>
-      <c r="F15" s="258"/>
-      <c r="G15" s="258"/>
-      <c r="H15" s="258"/>
-      <c r="I15" s="258"/>
-      <c r="J15" s="258"/>
-      <c r="K15" s="258"/>
-      <c r="L15" s="258"/>
-      <c r="M15" s="258"/>
-      <c r="N15" s="258"/>
-      <c r="O15" s="258"/>
-      <c r="P15" s="258"/>
-      <c r="Q15" s="258"/>
-      <c r="R15" s="259"/>
+      <c r="B15" s="260"/>
+      <c r="C15" s="260"/>
+      <c r="D15" s="260"/>
+      <c r="E15" s="260"/>
+      <c r="F15" s="260"/>
+      <c r="G15" s="260"/>
+      <c r="H15" s="260"/>
+      <c r="I15" s="260"/>
+      <c r="J15" s="260"/>
+      <c r="K15" s="260"/>
+      <c r="L15" s="260"/>
+      <c r="M15" s="260"/>
+      <c r="N15" s="260"/>
+      <c r="O15" s="260"/>
+      <c r="P15" s="260"/>
+      <c r="Q15" s="260"/>
+      <c r="R15" s="261"/>
     </row>
     <row r="16" spans="1:18" ht="33" customHeight="1">
-      <c r="A16" s="255" t="s">
+      <c r="A16" s="253" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="255" t="s">
+      <c r="B16" s="253" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="255" t="s">
+      <c r="C16" s="253" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="255" t="s">
+      <c r="D16" s="253" t="s">
         <v>164</v>
       </c>
-      <c r="E16" s="252" t="s">
+      <c r="E16" s="257" t="s">
         <v>208</v>
       </c>
-      <c r="F16" s="253"/>
-      <c r="G16" s="254"/>
-      <c r="H16" s="255" t="s">
+      <c r="F16" s="262"/>
+      <c r="G16" s="258"/>
+      <c r="H16" s="253" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="261" t="s">
+      <c r="I16" s="255" t="s">
         <v>211</v>
       </c>
-      <c r="J16" s="262"/>
-      <c r="K16" s="252" t="s">
+      <c r="J16" s="256"/>
+      <c r="K16" s="257" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="254"/>
-      <c r="M16" s="252" t="s">
+      <c r="L16" s="258"/>
+      <c r="M16" s="257" t="s">
         <v>213</v>
       </c>
-      <c r="N16" s="254"/>
+      <c r="N16" s="258"/>
       <c r="O16" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="P16" s="251" t="s">
+      <c r="P16" s="252" t="s">
         <v>214</v>
       </c>
-      <c r="Q16" s="251"/>
-      <c r="R16" s="260" t="s">
+      <c r="Q16" s="252"/>
+      <c r="R16" s="251" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="33" customHeight="1">
-      <c r="A17" s="256"/>
-      <c r="B17" s="256"/>
-      <c r="C17" s="256"/>
-      <c r="D17" s="256"/>
+      <c r="A17" s="254"/>
+      <c r="B17" s="254"/>
+      <c r="C17" s="254"/>
+      <c r="D17" s="254"/>
       <c r="E17" s="101" t="s">
         <v>205</v>
       </c>
@@ -6636,7 +6660,7 @@
       <c r="G17" s="101" t="s">
         <v>207</v>
       </c>
-      <c r="H17" s="256"/>
+      <c r="H17" s="254"/>
       <c r="I17" s="99" t="s">
         <v>135</v>
       </c>
@@ -6662,7 +6686,7 @@
       <c r="Q17" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="R17" s="260"/>
+      <c r="R17" s="251"/>
     </row>
     <row r="18" spans="1:18" ht="21" customHeight="1">
       <c r="A18" s="59" t="s">
@@ -6754,6 +6778,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:Q4"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A9:R9"/>
+    <mergeCell ref="R10:R11"/>
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="C10:C11"/>
@@ -6769,16 +6803,6 @@
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="A4:Q4"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A9:R9"/>
-    <mergeCell ref="R10:R11"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:L14 K18:L21">
@@ -11124,34 +11148,34 @@
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1"/>
     <row r="6" spans="1:14" ht="13.5" customHeight="1">
-      <c r="A6" s="204" t="s">
+      <c r="A6" s="202" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="205"/>
+      <c r="B6" s="203"/>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="210" t="s">
         <v>569</v>
       </c>
-      <c r="B7" s="207"/>
-      <c r="C7" s="206"/>
-      <c r="D7" s="206"/>
+      <c r="B7" s="210"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
       <c r="E7" s="74"/>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A8" s="208" t="s">
+      <c r="A8" s="211" t="s">
         <v>570</v>
       </c>
-      <c r="B8" s="208"/>
-      <c r="C8" s="206"/>
-      <c r="D8" s="206"/>
+      <c r="B8" s="211"/>
+      <c r="C8" s="209"/>
+      <c r="D8" s="209"/>
       <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A9" s="209" t="s">
+      <c r="A9" s="204" t="s">
         <v>571</v>
       </c>
-      <c r="B9" s="209"/>
+      <c r="B9" s="204"/>
       <c r="C9" s="111"/>
       <c r="D9" s="111"/>
       <c r="E9" s="111"/>
@@ -11160,10 +11184,10 @@
       <c r="I10" s="66"/>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A11" s="204" t="s">
+      <c r="A11" s="202" t="s">
         <v>476</v>
       </c>
-      <c r="B11" s="205"/>
+      <c r="B11" s="203"/>
     </row>
     <row r="12" spans="1:14" ht="33.75" customHeight="1">
       <c r="A12" s="77" t="s">
@@ -11192,16 +11216,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A13" s="202" t="s">
+      <c r="A13" s="205" t="s">
         <v>577</v>
       </c>
-      <c r="B13" s="202"/>
-      <c r="C13" s="202"/>
-      <c r="D13" s="202"/>
-      <c r="E13" s="202"/>
-      <c r="F13" s="202"/>
-      <c r="G13" s="202"/>
-      <c r="H13" s="203"/>
+      <c r="B13" s="205"/>
+      <c r="C13" s="205"/>
+      <c r="D13" s="205"/>
+      <c r="E13" s="205"/>
+      <c r="F13" s="205"/>
+      <c r="G13" s="205"/>
+      <c r="H13" s="206"/>
     </row>
     <row r="14" spans="1:14" ht="50.25" customHeight="1">
       <c r="A14" s="144" t="s">
@@ -11613,16 +11637,16 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A29" s="202" t="s">
+      <c r="A29" s="205" t="s">
         <v>669</v>
       </c>
-      <c r="B29" s="202"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="202"/>
-      <c r="E29" s="202"/>
-      <c r="F29" s="202"/>
-      <c r="G29" s="202"/>
-      <c r="H29" s="203"/>
+      <c r="B29" s="205"/>
+      <c r="C29" s="205"/>
+      <c r="D29" s="205"/>
+      <c r="E29" s="205"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
+      <c r="H29" s="206"/>
     </row>
     <row r="30" spans="1:14" ht="50.25" customHeight="1">
       <c r="A30" s="141" t="s">
@@ -11918,16 +11942,16 @@
       <c r="N39" s="23"/>
     </row>
     <row r="40" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A40" s="202" t="s">
+      <c r="A40" s="205" t="s">
         <v>659</v>
       </c>
-      <c r="B40" s="202"/>
-      <c r="C40" s="202"/>
-      <c r="D40" s="202"/>
-      <c r="E40" s="202"/>
-      <c r="F40" s="202"/>
-      <c r="G40" s="202"/>
-      <c r="H40" s="203"/>
+      <c r="B40" s="205"/>
+      <c r="C40" s="205"/>
+      <c r="D40" s="205"/>
+      <c r="E40" s="205"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
+      <c r="H40" s="206"/>
     </row>
     <row r="41" spans="1:14" ht="50.25" customHeight="1">
       <c r="A41" s="144" t="s">
@@ -12552,16 +12576,16 @@
       <c r="N61" s="23"/>
     </row>
     <row r="62" spans="1:14" ht="50.25" customHeight="1">
-      <c r="A62" s="202" t="s">
+      <c r="A62" s="205" t="s">
         <v>368</v>
       </c>
-      <c r="B62" s="202"/>
-      <c r="C62" s="202"/>
-      <c r="D62" s="202"/>
-      <c r="E62" s="202"/>
-      <c r="F62" s="202"/>
-      <c r="G62" s="202"/>
-      <c r="H62" s="203"/>
+      <c r="B62" s="205"/>
+      <c r="C62" s="205"/>
+      <c r="D62" s="205"/>
+      <c r="E62" s="205"/>
+      <c r="F62" s="205"/>
+      <c r="G62" s="205"/>
+      <c r="H62" s="206"/>
     </row>
     <row r="63" spans="1:14" ht="50.25" customHeight="1">
       <c r="A63" s="144" t="s">
@@ -12855,16 +12879,16 @@
       <c r="N74" s="23"/>
     </row>
     <row r="75" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A75" s="210" t="s">
+      <c r="A75" s="207" t="s">
         <v>372</v>
       </c>
-      <c r="B75" s="210"/>
-      <c r="C75" s="210"/>
-      <c r="D75" s="210"/>
-      <c r="E75" s="210"/>
-      <c r="F75" s="210"/>
-      <c r="G75" s="210"/>
-      <c r="H75" s="211"/>
+      <c r="B75" s="207"/>
+      <c r="C75" s="207"/>
+      <c r="D75" s="207"/>
+      <c r="E75" s="207"/>
+      <c r="F75" s="207"/>
+      <c r="G75" s="207"/>
+      <c r="H75" s="208"/>
     </row>
     <row r="76" spans="1:14" ht="50.25" customHeight="1">
       <c r="A76" s="141" t="s">
@@ -13135,16 +13159,16 @@
       <c r="H86" s="14"/>
     </row>
     <row r="87" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A87" s="202" t="s">
+      <c r="A87" s="205" t="s">
         <v>371</v>
       </c>
-      <c r="B87" s="202"/>
-      <c r="C87" s="202"/>
-      <c r="D87" s="202"/>
-      <c r="E87" s="202"/>
-      <c r="F87" s="202"/>
-      <c r="G87" s="202"/>
-      <c r="H87" s="203"/>
+      <c r="B87" s="205"/>
+      <c r="C87" s="205"/>
+      <c r="D87" s="205"/>
+      <c r="E87" s="205"/>
+      <c r="F87" s="205"/>
+      <c r="G87" s="205"/>
+      <c r="H87" s="206"/>
     </row>
     <row r="88" spans="1:14" ht="50.25" customHeight="1">
       <c r="A88" s="141" t="s">
@@ -13214,10 +13238,10 @@
     </row>
     <row r="91" spans="1:14" ht="33" customHeight="1"/>
     <row r="92" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A92" s="204" t="s">
+      <c r="A92" s="202" t="s">
         <v>350</v>
       </c>
-      <c r="B92" s="205"/>
+      <c r="B92" s="203"/>
     </row>
     <row r="93" spans="1:14" ht="33.75" customHeight="1">
       <c r="A93" s="77" t="s">
@@ -13246,16 +13270,16 @@
       </c>
     </row>
     <row r="94" spans="1:14" ht="33.75" customHeight="1">
-      <c r="A94" s="202" t="s">
+      <c r="A94" s="205" t="s">
         <v>577</v>
       </c>
-      <c r="B94" s="202"/>
-      <c r="C94" s="202"/>
-      <c r="D94" s="202"/>
-      <c r="E94" s="202"/>
-      <c r="F94" s="202"/>
-      <c r="G94" s="202"/>
-      <c r="H94" s="203"/>
+      <c r="B94" s="205"/>
+      <c r="C94" s="205"/>
+      <c r="D94" s="205"/>
+      <c r="E94" s="205"/>
+      <c r="F94" s="205"/>
+      <c r="G94" s="205"/>
+      <c r="H94" s="206"/>
     </row>
     <row r="95" spans="1:14" ht="50.25" customHeight="1">
       <c r="A95" s="144" t="s">
@@ -13336,10 +13360,10 @@
       <c r="N97" s="23"/>
     </row>
     <row r="99" spans="1:14">
-      <c r="A99" s="204" t="s">
+      <c r="A99" s="202" t="s">
         <v>476</v>
       </c>
-      <c r="B99" s="205"/>
+      <c r="B99" s="203"/>
     </row>
     <row r="100" spans="1:14" ht="47.25">
       <c r="A100" s="77" t="s">
@@ -13368,16 +13392,16 @@
       </c>
     </row>
     <row r="101" spans="1:14">
-      <c r="A101" s="202" t="s">
+      <c r="A101" s="205" t="s">
         <v>577</v>
       </c>
-      <c r="B101" s="202"/>
-      <c r="C101" s="202"/>
-      <c r="D101" s="202"/>
-      <c r="E101" s="202"/>
-      <c r="F101" s="202"/>
-      <c r="G101" s="202"/>
-      <c r="H101" s="203"/>
+      <c r="B101" s="205"/>
+      <c r="C101" s="205"/>
+      <c r="D101" s="205"/>
+      <c r="E101" s="205"/>
+      <c r="F101" s="205"/>
+      <c r="G101" s="205"/>
+      <c r="H101" s="206"/>
     </row>
     <row r="102" spans="1:14" ht="30">
       <c r="A102" s="144" t="s">
@@ -13474,6 +13498,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
@@ -13486,12 +13516,6 @@
     <mergeCell ref="A62:H62"/>
     <mergeCell ref="A75:H75"/>
     <mergeCell ref="A87:H87"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E95:E97 E63:E74 E41:E61 E76:E86 E88:E90 E30:E39 E14:E28 E102:E105">
@@ -13637,7 +13661,7 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="F6:F8"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9">
       <formula1>GoalDependencyType</formula1>
     </dataValidation>

</xml_diff>